<commit_message>
Add Use Case diagram to the repository
</commit_message>
<xml_diff>
--- a/BLib_MindMap.xlsx
+++ b/BLib_MindMap.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Documents/Degree/5th Semester/BLib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1737" documentId="11_EA8E006AEBEA90CE8A160B26B3A35F314D8274F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6391366-73FE-40F6-8330-C577ECED30D2}"/>
+  <xr:revisionPtr revIDLastSave="1861" documentId="11_EA8E006AEBEA90CE8A160B26B3A35F314D8274F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFD920B4-5B90-4EEB-89E8-CDFBACD91FFD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="2" r:id="rId1"/>
-    <sheet name="Meeting Schedule" sheetId="5" r:id="rId2"/>
-    <sheet name="Code Standards" sheetId="4" r:id="rId3"/>
-    <sheet name="Requirements" sheetId="1" r:id="rId4"/>
-    <sheet name="Acceptance Testing" sheetId="3" r:id="rId5"/>
-    <sheet name="WBS " sheetId="6" r:id="rId6"/>
+    <sheet name="Team Roles " sheetId="7" r:id="rId2"/>
+    <sheet name="Meeting Schedule" sheetId="5" r:id="rId3"/>
+    <sheet name="Code Standards" sheetId="4" r:id="rId4"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId5"/>
+    <sheet name="Acceptance Testing" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +40,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F65DB051-A65E-44A4-A28C-7BA965ADD77C}</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{F65DB051-A65E-44A4-A28C-7BA965ADD77C}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    משוך נתונים על החברי צוות ותפקידים
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="335">
   <si>
     <t>Group No. 5</t>
   </si>
@@ -100,12 +119,6 @@
     <t>Requirements</t>
   </si>
   <si>
-    <t>תרגיל מס 1 ע. צוות.docx</t>
-  </si>
-  <si>
-    <t>יש להכניס שבוע של TODOLIST למטלה ולהגיש</t>
-  </si>
-  <si>
     <t>Acceptance Testing</t>
   </si>
   <si>
@@ -116,9 +129,6 @@
   </si>
   <si>
     <t>מטלה 1 שיטות (אינטנסיבית) - תיקיית הגשה</t>
-  </si>
-  <si>
-    <t>בוצע 1/4</t>
   </si>
   <si>
     <t>Useful links</t>
@@ -3459,118 +3469,115 @@
     <t>ENTER MORE INFORMATION AS NEEDED</t>
   </si>
   <si>
-    <r>
-      <t>WBS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – מבנה תכולת הפרויקט:</t>
-    </r>
-  </si>
-  <si>
-    <t>זיהוי פעילות</t>
-  </si>
-  <si>
-    <t>תיאור פעילות</t>
-  </si>
-  <si>
-    <t>פעילות קודמת</t>
-  </si>
-  <si>
-    <t>Role:</t>
-  </si>
-  <si>
-    <t>Full Name:</t>
-  </si>
-  <si>
     <t>Product Owner</t>
   </si>
   <si>
     <t>Yuval Kogan</t>
   </si>
   <si>
-    <t>Scrum Master</t>
-  </si>
-  <si>
     <t>Ron Salama</t>
   </si>
   <si>
-    <t>Analysis of the Software Requirements</t>
-  </si>
-  <si>
-    <t>Development environment preperation</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Use Case diagram with description</t>
-  </si>
-  <si>
-    <t>Class Diagram</t>
-  </si>
-  <si>
-    <t>Activity and Sequence Diagrams</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Acceptance Test</t>
-  </si>
-  <si>
     <t>עבודה על המטלה של שיטות הנדסיות + מטלה של ממשק אדם מחשב.</t>
   </si>
   <si>
-    <t>אחראי</t>
-  </si>
-  <si>
-    <t>זמן התחלה</t>
-  </si>
-  <si>
-    <t>זמן סיום</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>יובל + דניאל</t>
-  </si>
-  <si>
-    <t>רון + יניב</t>
-  </si>
-  <si>
-    <t>ליאור + אלמוג</t>
-  </si>
-  <si>
-    <t>דניאל + יניב</t>
-  </si>
-  <si>
-    <t>Task 1 - Team Collaboration</t>
-  </si>
-  <si>
-    <t>1+2</t>
-  </si>
-  <si>
     <t>Scrum master</t>
   </si>
   <si>
-    <t>Column2</t>
-  </si>
-  <si>
     <t>פגישה ב13:30 מגיעים לפחות 5 דקות לפני, קישור לזום יופיע פה.</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Almog Raz</t>
+  </si>
+  <si>
+    <t>Yaniv Bodaga</t>
+  </si>
+  <si>
+    <t>Daniel Lachmakov</t>
+  </si>
+  <si>
+    <t>Lior Dagash</t>
+  </si>
+  <si>
+    <t>תפקיד 1 - שיטות</t>
+  </si>
+  <si>
+    <t>תפקיד 2 - שיטות</t>
+  </si>
+  <si>
+    <t>תפקיד 1 - ממשק אדם - מחשב</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Lecturer Coordinator</t>
+  </si>
+  <si>
+    <t>Daniel will be responsible for meeting with lecturers to review progress, gather feedback, and ensure alignment with their expectations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding Standards Overseer
+</t>
+  </si>
+  <si>
+    <t>Task1 ToDoList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Logistics Manager
+</t>
+  </si>
+  <si>
+    <t>Use Case Visual Paradigm</t>
+  </si>
+  <si>
+    <t>Yaniv is responsible for overseeing the planning, coordination, and execution of all logistical aspects of the project.</t>
+  </si>
+  <si>
+    <t>UI/UX Designer</t>
+  </si>
+  <si>
+    <t>Almog is responsible for creating an intuitive and visually appealing user interface, ensuring a seamless user experience.</t>
+  </si>
+  <si>
+    <t>Assignment Coordinator</t>
+  </si>
+  <si>
+    <t>Ron will oversee and manage the submission of all assignments and tasks, ensuring deadlines are met and deliverables are properly submitted on time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuval will take charge of administrative tasks and oversee the product's development, ensuring that all requirements are met and aligning the project with business goals. </t>
+  </si>
+  <si>
+    <t>Lior is responsible for maintaining high standards in code quality, naming conventions, and documentation.</t>
+  </si>
+  <si>
+    <t>המשך עבודה על מטלה של שיטות הנדסיות 1 - סיימנו ToDoList וגם מסמך Scrum Management</t>
+  </si>
+  <si>
+    <t>בוצע 3/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Roles </t>
+  </si>
+  <si>
+    <t>Specifies roles for each team member.</t>
+  </si>
+  <si>
+    <t>Specifies the requirements for the library project - "Blib".</t>
+  </si>
+  <si>
+    <t>Specifies the Acceptence Testing needed for the library project - "Blib".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3677,39 +3684,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="26"/>
@@ -3896,7 +3870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4129,12 +4103,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4158,13 +4126,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4176,73 +4144,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="61">
     <dxf>
       <fill>
         <patternFill>
@@ -4335,306 +4249,25 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5179,52 +4812,68 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="יובל כוגן" id="{0020C943-DF8D-440E-A473-11A712E33C2F}" userId="S::Yuval.Kogan@e.braude.ac.il::84800d58-b30d-47a5-ab10-b809ec1844cc" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A2:C17" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="65" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="58" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="E2:I15" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C34" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A1:C34" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="15">
+  <autoFilter ref="A1:E7" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7DD096F3-29E7-44B9-8E03-74AE8B0EFB58}" name="Full Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{86460309-D719-48D5-BE5A-FED925E8C505}" name="תפקיד 1 - שיטות" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{47A50531-CD06-43C3-AF93-5FE6CE915387}" name="תפקיד 2 - שיטות" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{9327F458-CD94-484D-95E0-7A5C295651CA}" name="תפקיד 1 - ממשק אדם - מחשב" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{875991B2-2D2B-439E-AAE3-9B4D6238D1C7}" name="Comments" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C35" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:C35" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="44"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41">
   <autoFilter ref="A1:C38" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{250D87B3-0E0E-41F7-BADF-53EC76930D5E}" name="Specification"/>
     <tableColumn id="3" xr3:uid="{53542E77-0500-4A50-A0B6-226ADBB40CAE}" name="Details"/>
   </tableColumns>
@@ -5232,66 +4881,29 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:E58" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="37"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="A2:E34" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4D23B098-F943-4DA5-86EC-90B0F85CAFB5}" name="Table7" displayName="Table7" ref="O3:P5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="O3:P5" xr:uid="{4D23B098-F943-4DA5-86EC-90B0F85CAFB5}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FAE58B6A-3818-4916-A91A-F827B3E3F42F}" name="Role:" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{DE181404-081B-4AAE-AA49-781211B7B7C1}" name="Full Name:" dataDxfId="23"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AAA2E6C2-289B-460E-9137-B2365CC517CA}" name="Table510" displayName="Table510" ref="A2:F11" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
-  <autoFilter ref="A2:F11" xr:uid="{AAA2E6C2-289B-460E-9137-B2365CC517CA}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CA3C999E-0453-4160-88D2-685A3732131A}" name="זיהוי פעילות" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{70742861-525D-4B43-9BCB-1473E9D41B55}" name="תיאור פעילות" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{3D0DC54F-B5F6-480F-A05F-54F26F0EDB4B}" name="פעילות קודמת" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{24E21D89-3D0E-4424-82EF-4C5D873E09CD}" name="זמן התחלה" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{21E5FD96-8280-486C-8F7B-DB2721A7BE15}" name="זמן סיום" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{90E87A28-4AC7-4DEC-A2D1-D0788B563C10}" name="אחראי" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7ECFF79F-C831-4069-9660-6CAD3DC87AEF}" name="Table10" displayName="Table10" ref="H2:I4" totalsRowShown="0">
-  <autoFilter ref="H2:I4" xr:uid="{7ECFF79F-C831-4069-9660-6CAD3DC87AEF}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7CF4C844-7570-4FCD-BABD-649D8D95DF7A}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{282E2F03-509B-4442-8A36-CC9577C053C0}" name="Column2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A2:E34" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5582,13 +5194,22 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K2" dT="2024-11-27T06:56:30.52" personId="{0020C943-DF8D-440E-A473-11A712E33C2F}" id="{F65DB051-A65E-44A4-A28C-7BA965ADD77C}">
+    <text xml:space="preserve">משוך נתונים על החברי צוות ותפקידים
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E429A24-44E4-45FF-AD25-4F9463F77043}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5611,7 +5232,7 @@
       </c>
       <c r="G1" s="65">
         <f ca="1">TODAY()</f>
-        <v>45622</v>
+        <v>45625</v>
       </c>
       <c r="I1" s="61"/>
     </row>
@@ -5660,23 +5281,23 @@
       <c r="G3" s="61">
         <v>45635</v>
       </c>
-      <c r="H3" s="102" t="s">
-        <v>335</v>
+      <c r="H3" s="78" t="s">
+        <v>306</v>
       </c>
       <c r="I3" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>13</v>
+        <v>331</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>332</v>
       </c>
       <c r="E4" s="58" t="b">
         <v>0</v>
@@ -5692,40 +5313,36 @@
       </c>
       <c r="I4" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="61">
-        <v>45637</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="64">
-        <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>15</v>
-      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="61"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
-        <v>21</v>
+      <c r="A6" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>333</v>
+      </c>
       <c r="E6" s="58" t="b">
         <v>0</v>
       </c>
@@ -5734,13 +5351,13 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>334</v>
       </c>
       <c r="E7" s="58" t="b">
         <v>0</v>
@@ -5748,8 +5365,16 @@
       <c r="G7" s="61"/>
       <c r="I7" s="64"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="58" t="b">
         <v>0</v>
       </c>
@@ -5772,104 +5397,118 @@
         <v>0</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" s="61">
         <v>45629</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>25</v>
+        <v>330</v>
       </c>
       <c r="I10" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="46"/>
       <c r="E11" s="58" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="68" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>24</v>
       </c>
       <c r="G11" s="61">
         <v>45629</v>
       </c>
-      <c r="H11" s="78" t="s">
-        <v>28</v>
+      <c r="H11" s="76" t="s">
+        <v>25</v>
       </c>
       <c r="I11" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" s="58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="G12" s="61">
         <v>45629</v>
       </c>
-      <c r="H12" s="78" t="s">
-        <v>33</v>
+      <c r="H12" s="76" t="s">
+        <v>30</v>
       </c>
       <c r="I12" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="58" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="61"/>
-      <c r="I13" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="61">
+        <v>45629</v>
+      </c>
+      <c r="H13" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="64">
+        <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" s="58" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="G14" s="61"/>
       <c r="I14" s="64"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E15" s="58" t="b">
         <v>0</v>
@@ -5999,31 +5638,241 @@
     <hyperlink ref="A12" r:id="rId2" xr:uid="{4ADF0731-A866-4A04-AD4C-41CF7A55A650}"/>
     <hyperlink ref="A13" r:id="rId3" xr:uid="{D721E76C-C8DC-4808-A841-2F6EFE921BB4}"/>
     <hyperlink ref="A14" r:id="rId4" display="../../../../../../../:b:/g/personal/yuval_kogan_e_braude_ac_il/EfU_Sk6Jc31DqgewyVmyPz0BgZgmEikU0pvZqYcgU7Zo2A?e=DWPsfw" xr:uid="{EA24A45E-43D3-47FC-AEE3-912A674C0ACF}"/>
-    <hyperlink ref="A5" location="Requirements!A1" display="Requirements" xr:uid="{B345F7E3-5C77-4395-8C88-38DE93ACC275}"/>
-    <hyperlink ref="A6" location="'Acceptance Testing'!A1" display="Acceptance Testing" xr:uid="{3CCC46CF-6006-4698-9963-2725A4632619}"/>
-    <hyperlink ref="A7" location="'Code Standards'!A1" display="Code Standards" xr:uid="{E088CDC4-824C-4B01-B550-1E21BEDDA856}"/>
+    <hyperlink ref="A6" location="Requirements!A1" display="Requirements" xr:uid="{B345F7E3-5C77-4395-8C88-38DE93ACC275}"/>
+    <hyperlink ref="A7" location="'Acceptance Testing'!A1" display="Acceptance Testing" xr:uid="{3CCC46CF-6006-4698-9963-2725A4632619}"/>
+    <hyperlink ref="A8" location="'Code Standards'!A1" display="Code Standards" xr:uid="{E088CDC4-824C-4B01-B550-1E21BEDDA856}"/>
     <hyperlink ref="F3" r:id="rId5" xr:uid="{0CA81D24-ABF4-4FF7-B140-63A0E0868148}"/>
-    <hyperlink ref="F5" r:id="rId6" xr:uid="{1ABC11E3-A784-4609-8904-95844B51DA2B}"/>
-    <hyperlink ref="F4" r:id="rId7" xr:uid="{2BF54119-7B1D-444F-AFAD-37FE8145D2D1}"/>
-    <hyperlink ref="F11" r:id="rId8" display="../../../../../../../:w:/g/personal/yuval_kogan_e_braude_ac_il/EeyYJbL0CQlNp9PWd9rqSiIB1kJMqs02PpGsmhfyq2oIMA?e=FkL4N5" xr:uid="{D74B4050-7C9B-41FC-B168-0EC857577417}"/>
-    <hyperlink ref="F12" r:id="rId9" xr:uid="{4677B6FE-5532-4F16-96FB-FDEA1B667E3E}"/>
-    <hyperlink ref="F10" r:id="rId10" xr:uid="{6CFBD0B4-BDF8-4D4F-AD73-809DE1C60E6E}"/>
-    <hyperlink ref="A4" location="'Meeting Schedule'!A1" display="Meeting Schedule" xr:uid="{9F408324-F2FC-4899-B497-74781498329D}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{2BF54119-7B1D-444F-AFAD-37FE8145D2D1}"/>
+    <hyperlink ref="F11" r:id="rId7" display="../../../../../../../:w:/g/personal/yuval_kogan_e_braude_ac_il/EeyYJbL0CQlNp9PWd9rqSiIB1kJMqs02PpGsmhfyq2oIMA?e=FkL4N5" xr:uid="{D74B4050-7C9B-41FC-B168-0EC857577417}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{4677B6FE-5532-4F16-96FB-FDEA1B667E3E}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{6CFBD0B4-BDF8-4D4F-AD73-809DE1C60E6E}"/>
+    <hyperlink ref="A5" location="'Meeting Schedule'!A1" display="Meeting Schedule" xr:uid="{9F408324-F2FC-4899-B497-74781498329D}"/>
+    <hyperlink ref="A4" location="'Team Roles '!A1" display="Team Roles " xr:uid="{CB85ACBE-0077-476A-9693-F18F6AAA8680}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
+    <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
-    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538DB23-0864-46D9-82F7-B6A0E6DA13F2}">
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE753598-B63F-4BFF-A796-9131C2B9321B}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" style="79" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="79" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="79" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.5703125" style="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="79"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+    </row>
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="80" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="80" t="s">
+        <v>324</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="80" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="80" t="s">
+        <v>317</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="80" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="80" t="s">
+        <v>328</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538DB23-0864-46D9-82F7-B6A0E6DA13F2}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6034,209 +5883,218 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="79">
+      <c r="A2" s="77">
         <v>45617</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="79">
+      <c r="A3" s="77">
         <v>45619</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="79">
+      <c r="A4" s="77">
         <v>45622</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="79">
+      <c r="A5" s="77">
+        <v>45624</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="77">
         <v>45629</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="79">
-        <v>45636</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="79">
-        <v>45643</v>
+      <c r="A7" s="77">
+        <v>45636</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="79">
-        <v>45650</v>
+      <c r="A8" s="77">
+        <v>45643</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="79">
-        <v>45657</v>
+      <c r="A9" s="77">
+        <v>45650</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="79">
-        <v>45664</v>
+      <c r="A10" s="77">
+        <v>45657</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="79">
-        <v>45671</v>
+      <c r="A11" s="77">
+        <v>45664</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="79">
-        <v>45678</v>
+      <c r="A12" s="77">
+        <v>45671</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="79">
-        <v>45685</v>
+      <c r="A13" s="77">
+        <v>45678</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
+      <c r="A14" s="77">
+        <v>45685</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="77"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
+      <c r="A19" s="77"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
+      <c r="A20" s="77"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
+      <c r="A23" s="77"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="79"/>
+      <c r="A24" s="77"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="79"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
+      <c r="A27" s="77"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
+      <c r="A28" s="77"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
+      <c r="A30" s="77"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="79"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="77"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6246,7 +6104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0F8AA7-3D0F-4359-84F6-848A1B337549}">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -6263,420 +6121,420 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
-        <v>102</v>
-      </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
         <v>117</v>
       </c>
-      <c r="B35" t="s">
-        <v>120</v>
-      </c>
       <c r="C35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
         <v>122</v>
       </c>
-      <c r="B37" t="s">
-        <v>125</v>
-      </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -6687,13 +6545,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6708,26 +6566,26 @@
   <sheetData>
     <row r="1" spans="1:46" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:46" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -6781,10 +6639,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="b">
@@ -6796,10 +6654,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="b">
@@ -6811,10 +6669,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16" t="b">
@@ -6826,10 +6684,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="b">
@@ -6841,10 +6699,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="b">
@@ -6856,10 +6714,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="b">
@@ -6871,10 +6729,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16" t="b">
@@ -6925,7 +6783,7 @@
     <row r="10" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -6938,10 +6796,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="20"/>
@@ -6951,10 +6809,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="b">
@@ -7007,10 +6865,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16" t="b">
@@ -7063,10 +6921,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="b">
@@ -7078,10 +6936,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16" t="b">
@@ -7132,7 +6990,7 @@
     <row r="16" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -7145,10 +7003,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16" t="b">
@@ -7160,10 +7018,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="b">
@@ -7174,14 +7032,14 @@
       <c r="A19" s="14">
         <v>15</v>
       </c>
-      <c r="B19" s="70" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="72" t="b">
+      <c r="B19" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7190,10 +7048,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16" t="b">
@@ -7205,10 +7063,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16" t="b">
@@ -7220,10 +7078,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="b">
@@ -7235,10 +7093,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16" t="b">
@@ -7250,10 +7108,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="b">
@@ -7265,10 +7123,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="b">
@@ -7280,10 +7138,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16" t="b">
@@ -7295,10 +7153,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16" t="b">
@@ -7310,10 +7168,10 @@
         <v>24</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16" t="b">
@@ -7366,10 +7224,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="b">
@@ -7422,10 +7280,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16" t="b">
@@ -7437,10 +7295,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16" t="b">
@@ -7450,7 +7308,7 @@
     <row r="32" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -7463,10 +7321,10 @@
         <v>27</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="16" t="b">
@@ -7478,10 +7336,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="16" t="b">
@@ -7493,13 +7351,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E35" s="16" t="b">
         <v>0</v>
@@ -7510,10 +7368,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16" t="b">
@@ -7525,10 +7383,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="16" t="b">
@@ -7540,10 +7398,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="16" t="b">
@@ -7596,10 +7454,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="16" t="b">
@@ -7611,10 +7469,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16" t="b">
@@ -7624,7 +7482,7 @@
     <row r="41" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -7637,10 +7495,10 @@
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="16" t="b">
@@ -7693,10 +7551,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="16" t="b">
@@ -7708,13 +7566,13 @@
         <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E44" s="16" t="b">
         <v>0</v>
@@ -7723,7 +7581,7 @@
     <row r="45" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -7736,10 +7594,10 @@
         <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16" t="b">
@@ -7751,10 +7609,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="16" t="b">
@@ -7766,13 +7624,13 @@
         <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E48" s="16" t="b">
         <v>0</v>
@@ -7783,10 +7641,10 @@
         <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="16" t="b">
@@ -7839,13 +7697,13 @@
         <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E50" s="16" t="b">
         <v>0</v>
@@ -7856,10 +7714,10 @@
         <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16" t="b">
@@ -7869,7 +7727,7 @@
     <row r="52" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -7882,13 +7740,13 @@
         <v>44</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E53" s="16" t="b">
         <v>0</v>
@@ -7899,10 +7757,10 @@
         <v>45</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16" t="b">
@@ -7914,13 +7772,13 @@
         <v>46</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E55" s="16" t="b">
         <v>0</v>
@@ -7931,13 +7789,13 @@
         <v>47</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E56" s="28" t="b">
         <v>0</v>
@@ -7947,11 +7805,11 @@
       <c r="A57" s="26">
         <v>48</v>
       </c>
-      <c r="B57" s="73" t="s">
-        <v>198</v>
+      <c r="B57" s="71" t="s">
+        <v>195</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="28" t="b">
@@ -7962,11 +7820,11 @@
       <c r="A58" s="26">
         <v>49</v>
       </c>
-      <c r="B58" s="73" t="s">
-        <v>199</v>
+      <c r="B58" s="71" t="s">
+        <v>196</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="28" t="b">
@@ -7989,7 +7847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E2CEC-5E0E-48DE-BE54-48780618BFB0}">
   <dimension ref="A1:O35"/>
   <sheetViews>
@@ -8014,7 +7872,7 @@
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
       <c r="B1" s="42" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -8022,164 +7880,164 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="E2" s="33" t="s">
         <v>201</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>205</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>208</v>
       </c>
       <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:8" ht="318.75" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="D6" s="34" t="s">
         <v>214</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>217</v>
       </c>
       <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>222</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>225</v>
       </c>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D9" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>225</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="39" t="s">
         <v>229</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E11" s="39"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -8189,14 +8047,14 @@
     </row>
     <row r="14" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="36"/>
@@ -8205,19 +8063,19 @@
     </row>
     <row r="15" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>239</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>242</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -8225,19 +8083,19 @@
     </row>
     <row r="16" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E16" s="39" t="s">
         <v>243</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>246</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -8245,294 +8103,294 @@
     </row>
     <row r="17" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" s="39" t="s">
         <v>247</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" s="39" t="s">
         <v>251</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="262.5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="B19" s="75" t="s">
-        <v>256</v>
+        <v>252</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>253</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="B20" s="75" t="s">
-        <v>259</v>
+        <v>255</v>
+      </c>
+      <c r="B20" s="73" t="s">
+        <v>256</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B21" s="76" t="s">
-        <v>261</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>263</v>
-      </c>
       <c r="E21" s="39" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="D22" s="34" t="s">
         <v>264</v>
-      </c>
-      <c r="B22" s="75" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>267</v>
       </c>
       <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="34" t="s">
         <v>268</v>
-      </c>
-      <c r="B23" s="75" t="s">
-        <v>269</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>271</v>
       </c>
       <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
-        <v>272</v>
-      </c>
-      <c r="B24" s="75" t="s">
-        <v>273</v>
+        <v>269</v>
+      </c>
+      <c r="B24" s="73" t="s">
+        <v>270</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>275</v>
-      </c>
-      <c r="B25" s="75" t="s">
-        <v>276</v>
+        <v>272</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>273</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="B26" s="75" t="s">
-        <v>278</v>
+        <v>274</v>
+      </c>
+      <c r="B26" s="73" t="s">
+        <v>275</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:15" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="D27" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="E27" s="39" t="s">
         <v>281</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>282</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>283</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="B28" s="75" t="s">
+        <v>282</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="E28" s="39" t="s">
         <v>281</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>287</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="236.25" x14ac:dyDescent="0.5">
       <c r="A29" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="O29" s="72" t="s">
         <v>288</v>
-      </c>
-      <c r="B29" s="75" t="s">
-        <v>281</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>290</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>284</v>
-      </c>
-      <c r="O29" s="74" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="B30" s="75" t="s">
-        <v>281</v>
+        <v>289</v>
+      </c>
+      <c r="B30" s="73" t="s">
+        <v>278</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="39" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="77"/>
+      <c r="E31" s="75"/>
     </row>
     <row r="32" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B34" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="D34" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="C34" s="41" t="s">
-        <v>300</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>302</v>
-      </c>
       <c r="E34" s="39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="37" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -8573,606 +8431,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDC2E9D-CECB-44FE-A57D-FD3AD31EFC03}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:P51"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81"/>
-      <c r="B1" s="80" t="s">
-        <v>304</v>
-      </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="81"/>
-    </row>
-    <row r="2" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
-        <v>305</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" s="89" t="s">
-        <v>307</v>
-      </c>
-      <c r="D2" s="89" t="s">
-        <v>324</v>
-      </c>
-      <c r="E2" s="89" t="s">
-        <v>325</v>
-      </c>
-      <c r="F2" s="90" t="s">
-        <v>323</v>
-      </c>
-      <c r="H2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="91">
-        <v>1</v>
-      </c>
-      <c r="B3" s="92" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="93" t="s">
-        <v>217</v>
-      </c>
-      <c r="D3" s="94">
-        <v>21.11</v>
-      </c>
-      <c r="E3" s="93">
-        <v>23.11</v>
-      </c>
-      <c r="F3" s="95" t="s">
-        <v>327</v>
-      </c>
-      <c r="H3" t="s">
-        <v>333</v>
-      </c>
-      <c r="I3" t="s">
-        <v>313</v>
-      </c>
-      <c r="O3" s="66" t="s">
-        <v>308</v>
-      </c>
-      <c r="P3" s="66" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="91">
-        <v>2</v>
-      </c>
-      <c r="B4" s="92" t="s">
-        <v>317</v>
-      </c>
-      <c r="C4" s="93">
-        <v>1</v>
-      </c>
-      <c r="D4" s="94">
-        <v>24.11</v>
-      </c>
-      <c r="E4" s="93">
-        <v>25.11</v>
-      </c>
-      <c r="F4" s="95" t="s">
-        <v>328</v>
-      </c>
-      <c r="H4" t="s">
-        <v>310</v>
-      </c>
-      <c r="I4" t="s">
-        <v>311</v>
-      </c>
-      <c r="O4" s="66" t="s">
-        <v>310</v>
-      </c>
-      <c r="P4" s="67" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="91">
-        <v>3</v>
-      </c>
-      <c r="B5" s="92" t="s">
-        <v>321</v>
-      </c>
-      <c r="C5" s="93" t="s">
-        <v>332</v>
-      </c>
-      <c r="D5" s="94">
-        <v>26.11</v>
-      </c>
-      <c r="E5" s="93">
-        <v>27.11</v>
-      </c>
-      <c r="F5" s="95" t="s">
-        <v>329</v>
-      </c>
-      <c r="O5" s="66" t="s">
-        <v>312</v>
-      </c>
-      <c r="P5" s="66" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="91">
-        <v>4</v>
-      </c>
-      <c r="B6" s="92" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="93">
-        <v>3</v>
-      </c>
-      <c r="D6" s="94">
-        <v>28.11</v>
-      </c>
-      <c r="E6" s="93">
-        <v>30.11</v>
-      </c>
-      <c r="F6" s="95" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="91">
-        <v>5</v>
-      </c>
-      <c r="B7" s="94" t="s">
-        <v>331</v>
-      </c>
-      <c r="C7" s="93">
-        <v>4</v>
-      </c>
-      <c r="D7" s="94">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E7" s="93">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="F7" s="95" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="91">
-        <v>6</v>
-      </c>
-      <c r="B8" s="92" t="s">
-        <v>316</v>
-      </c>
-      <c r="C8" s="93">
-        <v>5</v>
-      </c>
-      <c r="D8" s="94">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="E8" s="93">
-        <v>10.119999999999999</v>
-      </c>
-      <c r="F8" s="95" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="91">
-        <v>7</v>
-      </c>
-      <c r="B9" s="92" t="s">
-        <v>320</v>
-      </c>
-      <c r="C9" s="93">
-        <v>5</v>
-      </c>
-      <c r="D9" s="94">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="E9" s="93">
-        <v>10.119999999999999</v>
-      </c>
-      <c r="F9" s="95" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="91">
-        <v>8</v>
-      </c>
-      <c r="B10" s="92" t="s">
-        <v>319</v>
-      </c>
-      <c r="C10" s="93">
-        <v>6</v>
-      </c>
-      <c r="D10" s="94">
-        <v>11.12</v>
-      </c>
-      <c r="E10" s="93">
-        <v>13.12</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="96">
-        <v>9</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>318</v>
-      </c>
-      <c r="C11" s="98">
-        <v>6</v>
-      </c>
-      <c r="D11" s="97">
-        <v>11.12</v>
-      </c>
-      <c r="E11" s="98">
-        <v>13.12</v>
-      </c>
-      <c r="F11" s="99" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="85"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="84"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="85"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="84"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="85"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="84"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="85"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="84"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="84"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="85"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="85"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="85"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="84"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="85"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="84"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="85"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="84"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="85"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="84"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="85"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="84"/>
-      <c r="B26" s="100"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="85"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="84"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="85"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="85"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="84"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="85"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="84"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="85"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="84"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="85"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="85"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="85"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="85"/>
-      <c r="B36" s="85"/>
-      <c r="C36" s="85"/>
-      <c r="D36" s="85"/>
-      <c r="E36" s="85"/>
-      <c r="F36" s="85"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="85"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="85"/>
-      <c r="B38" s="85"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="85"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="85"/>
-      <c r="B42" s="85"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="85"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
-      <c r="B43" s="85"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="85"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="85"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="85"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="85"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
-      <c r="B45" s="85"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="85"/>
-      <c r="D46" s="85"/>
-      <c r="E46" s="85"/>
-      <c r="F46" s="85"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="85"/>
-      <c r="B47" s="85"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="85"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="85"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="85"/>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="85"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="85"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add pom file for testing
</commit_message>
<xml_diff>
--- a/BLib_MindMap.xlsx
+++ b/BLib_MindMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Documents/Degree/5th Semester/BLib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2250" documentId="11_EA8E006AEBEA90CE8A160B26B3A35F314D8274F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0CF5D9B-7E49-4F24-8A10-382747615713}"/>
+  <xr:revisionPtr revIDLastSave="2318" documentId="11_EA8E006AEBEA90CE8A160B26B3A35F314D8274F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7739CE54-A389-4DCC-9C45-DC27908C28D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="382">
   <si>
     <t>Group No. 5</t>
   </si>
@@ -98,12 +98,6 @@
   <si>
     <t>Version Control
 Note: This file and UML diagrams are passed using the git repository.</t>
-  </si>
-  <si>
-    <t>ממשק אדם מחשב מטלה 1</t>
-  </si>
-  <si>
-    <t>פגישה ב13:30 מגיעים לפחות 5 דקות לפני, קישור לזום יופיע פה.</t>
   </si>
   <si>
     <t xml:space="preserve">Team Roles </t>
@@ -444,9 +438,6 @@
   </si>
   <si>
     <t>עבודה על גיט בחצי צוות</t>
-  </si>
-  <si>
-    <t>מפגש סדנה עם ג'וליה בנוגע למטלה 1 של ממשק אדם - מחשב</t>
   </si>
   <si>
     <t>Category</t>
@@ -3728,6 +3719,36 @@
   </si>
   <si>
     <t>יובל</t>
+  </si>
+  <si>
+    <t>יניב + אלמוג</t>
+  </si>
+  <si>
+    <t>יובל + ליאור</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רון </t>
+  </si>
+  <si>
+    <t>ברגע שמסיימים עם ה-Sequence עוברים ל-Class</t>
+  </si>
+  <si>
+    <t>רון</t>
+  </si>
+  <si>
+    <t>עבר בקרה?</t>
+  </si>
+  <si>
+    <t>מי עשה בקרה?</t>
+  </si>
+  <si>
+    <t>מפגש סדנה עם ג'וליה בנוגע למטלה 1 של ממשק אדם - מחשב + מפגש תיקון על המטלה</t>
+  </si>
+  <si>
+    <t>התחלת עבודה על מטלה 2 - שיטות הנדסיות, התחלת עבודה על UML</t>
+  </si>
+  <si>
+    <t>המשך עבודה על מטלה 2 של שיטות, המשך UML, התחלת בקרה על המטלה</t>
   </si>
 </sst>
 </file>
@@ -4039,7 +4060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4354,24 +4375,18 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="77">
     <dxf>
       <fill>
         <patternFill>
@@ -4924,22 +4939,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -5058,14 +5089,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>314324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -5132,39 +5163,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="A2:C17" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="72" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="74" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="E2:I15" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:F17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
-  <autoFilter ref="A1:F17" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:H17" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+  <autoFilter ref="A1:H17" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{6F08DEB8-9412-4A60-827F-650CE5DE012A}" name="מי עשה בקרה?" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{0B213265-848E-42AD-BB24-FACA108AE82B}" name="עבר בקרה?" dataDxfId="57"/>
     <tableColumn id="5" xr3:uid="{C212956F-6717-4ACE-9560-C2C858E916CC}" name="ניקוד במטלה" dataDxfId="56"/>
     <tableColumn id="6" xr3:uid="{4BAEA3F5-7A0E-45FC-BD15-78D20A6CE5AF}" name="הערות" dataDxfId="55"/>
   </tableColumns>
@@ -5173,8 +5206,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="H3:I7" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="H3:I7" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="J3:K7" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="J3:K7" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9D0FE680-0194-44E8-8173-C409E67F91A6}" name="קישור" dataDxfId="52"/>
     <tableColumn id="2" xr3:uid="{4D3F5656-E6FB-49EB-ACFD-772E84A9C306}" name="הסבר" dataDxfId="51"/>
@@ -5198,8 +5231,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C38" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:C38" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C39" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:C39" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="40"/>
@@ -5547,37 +5580,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E429A24-44E4-45FF-AD25-4F9463F77043}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2"/>
-    <col min="5" max="5" width="9.5703125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="2"/>
+    <col min="5" max="5" width="9.5546875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.28515625" style="2"/>
+    <col min="10" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="65">
         <f ca="1">TODAY()</f>
-        <v>45636</v>
+        <v>45637</v>
       </c>
       <c r="I1" s="61"/>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
@@ -5603,7 +5636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
@@ -5614,58 +5647,49 @@
         <v>11</v>
       </c>
       <c r="E3" s="58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="61">
-        <v>45635</v>
-      </c>
-      <c r="H3" s="77" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="64">
-        <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="58" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="61">
         <v>45650</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="58" t="b">
         <v>0</v>
@@ -5674,15 +5698,15 @@
       <c r="G5" s="61"/>
       <c r="I5" s="64"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="58" t="b">
         <v>0</v>
@@ -5690,15 +5714,15 @@
       <c r="G6" s="61"/>
       <c r="I6" s="64"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="58" t="b">
         <v>0</v>
@@ -5706,15 +5730,15 @@
       <c r="G7" s="61"/>
       <c r="I7" s="64"/>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="58" t="b">
         <v>0</v>
@@ -5722,7 +5746,7 @@
       <c r="G8" s="61"/>
       <c r="I8" s="64"/>
     </row>
-    <row r="9" spans="1:9" s="47" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5732,7 +5756,7 @@
       <c r="G9" s="62"/>
       <c r="I9" s="64"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="E10" s="58" t="b">
         <v>0</v>
@@ -5741,10 +5765,10 @@
       <c r="G10" s="61"/>
       <c r="I10" s="64"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="46"/>
       <c r="E11" s="58" t="b">
@@ -5754,12 +5778,12 @@
       <c r="G11" s="61"/>
       <c r="I11" s="64"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="58" t="b">
         <v>0</v>
@@ -5767,15 +5791,15 @@
       <c r="G12" s="61"/>
       <c r="I12" s="64"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E13" s="58" t="b">
         <v>0</v>
@@ -5784,15 +5808,15 @@
       <c r="G13" s="61"/>
       <c r="I13" s="64"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="58" t="b">
         <v>0</v>
@@ -5800,108 +5824,108 @@
       <c r="G14" s="61"/>
       <c r="I14" s="64"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="58" t="b">
         <v>0</v>
       </c>
       <c r="G15" s="61"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
       <c r="G16" s="61"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="G17" s="63"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G18" s="61"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G19" s="61"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G20" s="61"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G21" s="61"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G22" s="61"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G23" s="61"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G24" s="61"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G25" s="61"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G26" s="61"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G27" s="61"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G28" s="61"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G29" s="61"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G30" s="61"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G31" s="61"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G32" s="61"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" s="61"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" s="61"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" s="61"/>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" s="61"/>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" s="61"/>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G38" s="61"/>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G39" s="61"/>
     </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G40" s="61"/>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G41" s="61"/>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G42" s="61"/>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G43" s="61"/>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G44" s="61"/>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G45" s="61"/>
     </row>
   </sheetData>
@@ -5938,16 +5962,15 @@
     <hyperlink ref="A6" location="Requirements!A1" display="Requirements" xr:uid="{B345F7E3-5C77-4395-8C88-38DE93ACC275}"/>
     <hyperlink ref="A7" location="'Acceptance Testing'!A1" display="Acceptance Testing" xr:uid="{3CCC46CF-6006-4698-9963-2725A4632619}"/>
     <hyperlink ref="A8" location="'Code Standards'!A1" display="Code Standards" xr:uid="{E088CDC4-824C-4B01-B550-1E21BEDDA856}"/>
-    <hyperlink ref="F3" r:id="rId5" xr:uid="{0CA81D24-ABF4-4FF7-B140-63A0E0868148}"/>
     <hyperlink ref="A5" location="'Meeting Schedule'!A1" display="Meeting Schedule" xr:uid="{9F408324-F2FC-4899-B497-74781498329D}"/>
     <hyperlink ref="A4" location="'Team Roles '!A1" display="Team Roles " xr:uid="{CB85ACBE-0077-476A-9693-F18F6AAA8680}"/>
-    <hyperlink ref="F4" r:id="rId6" xr:uid="{3D2C267D-39D7-41AD-AC19-90EEA685B986}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{3D2C267D-39D7-41AD-AC19-90EEA685B986}"/>
     <hyperlink ref="H4" location="'Task2 - Engineering Methods'!A1" display="חלוקת עבודה (לשונית Task2 - Engineering Methods)" xr:uid="{B9A29EFC-882A-4553-B64B-875D982E4977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
+    <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5957,347 +5980,452 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="79" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="86" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="79" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="79" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="79" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" style="87" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="79"/>
-    <col min="8" max="8" width="20.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" style="80" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="79"/>
-    <col min="11" max="11" width="14" style="79" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="79" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="79"/>
+    <col min="1" max="1" width="19.6640625" style="79" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="79" customWidth="1"/>
+    <col min="7" max="7" width="16" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" style="87" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="87" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" style="80" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="79"/>
+    <col min="13" max="13" width="14" style="79" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="79"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="85" t="s">
+        <v>378</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="83" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="85"/>
+      <c r="J1" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="83" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="84"/>
       <c r="C2" s="81" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="88"/>
-      <c r="H2" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="83" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="86" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="D3" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="1"/>
+      <c r="F3" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>18</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="H3" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="85"/>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="80" t="s">
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="B4" s="86" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D4" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="85"/>
+      <c r="J4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="K4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="89" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="77" t="s">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="93" t="s">
+      <c r="B5" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="D5" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="1"/>
+      <c r="F5" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>30</v>
       </c>
-      <c r="F5" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="90" t="s">
+      <c r="H5" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="85"/>
+      <c r="J5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="80" t="s">
+      <c r="B6" s="86" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="D6" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="1"/>
+      <c r="F6" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
         <v>12</v>
       </c>
-      <c r="F6" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="85"/>
+      <c r="J6" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="80" t="s">
+      <c r="B7" s="86" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D7" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="85"/>
+      <c r="J7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="89" t="b">
+      <c r="B8" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F8" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="80" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="86" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="89" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <v>5</v>
       </c>
-      <c r="F8" s="85" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H8" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="85"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="84"/>
       <c r="C9" s="81" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="88"/>
-      <c r="H9" s="92">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="91">
         <f ca="1">'Important Information'!I4</f>
-        <v>14</v>
-      </c>
-      <c r="I9" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="86" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="86" t="s">
-        <v>70</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1"/>
+      <c r="F10" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
         <v>25</v>
       </c>
-      <c r="F10" s="85"/>
-    </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+    </row>
+    <row r="11" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="86" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="89" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="85"/>
-    </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="F11" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+    </row>
+    <row r="12" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="86" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="89" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="85"/>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+    </row>
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" s="86" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="89" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="85"/>
-    </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="F13" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+    </row>
+    <row r="14" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="89" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="86" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="86"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="84"/>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="88"/>
-    </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="85"/>
+    </row>
+    <row r="16" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="86" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D16" s="89" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="1"/>
+      <c r="F16" s="89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
         <v>10</v>
       </c>
-      <c r="F16" s="85"/>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+    </row>
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="D17" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F17" s="89" t="b">
         <v>0</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="85"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="85"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C30" s="80"/>
     </row>
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
-  <conditionalFormatting sqref="D3:D8 D10:D14 D16:D17">
+  <conditionalFormatting sqref="D3:D8 F3:F8 D10:D14 F10:F14 D16:D17 F16:F17">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -6306,10 +6434,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="../../../../../../../:b:/g/personal/yuval_kogan_e_braude_ac_il/EfU_Sk6Jc31DqgewyVmyPz0BgZgmEikU0pvZqYcgU7Zo2A?e=DWPsfw" xr:uid="{BBE518CB-8073-43E8-9437-83ADD7890456}"/>
-    <hyperlink ref="H1" r:id="rId2" xr:uid="{4A71897C-0E71-4D69-9339-E03DF5D3265C}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{95EB343E-243E-4A1E-A51B-853D9E33ABF8}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{B0AF636B-F209-4C52-9425-536365A5B6E3}"/>
+    <hyperlink ref="J2" r:id="rId1" display="../../../../../../../:b:/g/personal/yuval_kogan_e_braude_ac_il/EfU_Sk6Jc31DqgewyVmyPz0BgZgmEikU0pvZqYcgU7Zo2A?e=DWPsfw" xr:uid="{BBE518CB-8073-43E8-9437-83ADD7890456}"/>
+    <hyperlink ref="J1" r:id="rId2" xr:uid="{4A71897C-0E71-4D69-9339-E03DF5D3265C}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{95EB343E-243E-4A1E-A51B-853D9E33ABF8}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{CDB1771F-18A8-4A96-BC17-764B808E14DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>
@@ -6328,113 +6456,113 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="78" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="78" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -6448,261 +6576,272 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538DB23-0864-46D9-82F7-B6A0E6DA13F2}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="75.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="76">
         <v>45617</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="76">
         <v>45619</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="76">
         <v>45622</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="76">
         <v>45624</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="76">
         <v>45625</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="76">
         <v>45628</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="76">
         <v>45630</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="76">
         <v>45635</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>115</v>
+        <v>379</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="76">
         <v>45636</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="76">
+        <v>45638</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="76">
         <v>45643</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="76">
-        <v>45650</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="76">
-        <v>45657</v>
+        <v>45650</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="76">
-        <v>45664</v>
+        <v>45657</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="76">
-        <v>45671</v>
+        <v>45664</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="76">
-        <v>45678</v>
+        <v>45671</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="76">
-        <v>45685</v>
+        <v>45678</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="76"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="76">
+        <v>45685</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="76"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="76"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="76"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="76"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="76"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="76"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="76"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="76"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="76"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="76"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="76"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="76"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="76"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="76"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="76"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="76"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="76"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="76"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="76"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="76"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="76"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6720,429 +6859,429 @@
       <selection activeCell="C13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
         <v>119</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>120</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>124</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>126</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>128</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="56" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>130</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
         <v>132</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>133</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>135</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>137</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>139</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="55" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>141</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
         <v>143</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" t="s">
         <v>144</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
         <v>146</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
         <v>148</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
         <v>150</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
         <v>152</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="56" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
         <v>156</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C20" t="s">
         <v>157</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>159</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="55" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" t="s">
         <v>161</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" t="s">
         <v>163</v>
       </c>
-      <c r="B22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
-        <v>163</v>
-      </c>
-      <c r="B23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>166</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>168</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" t="s">
         <v>170</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C27" t="s">
         <v>171</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
         <v>173</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
         <v>175</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>177</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" t="s">
         <v>179</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C31" t="s">
         <v>180</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C32" t="s">
         <v>182</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
         <v>184</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="56" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>186</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" t="s">
         <v>188</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>189</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>191</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" t="s">
         <v>193</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>194</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>196</v>
-      </c>
-      <c r="C37" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="B38" t="s">
-        <v>198</v>
-      </c>
-      <c r="C38" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7162,38 +7301,38 @@
       <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>204</v>
-      </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:46" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -7242,105 +7381,105 @@
       <c r="AS2" s="1"/>
       <c r="AT2" s="1"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16" t="b">
@@ -7388,10 +7527,10 @@
       <c r="AS9" s="1"/>
       <c r="AT9" s="1"/>
     </row>
-    <row r="10" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7399,28 +7538,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="b">
@@ -7468,15 +7607,15 @@
       <c r="AS12" s="1"/>
       <c r="AT12" s="1"/>
     </row>
-    <row r="13" spans="1:46" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16" t="b">
@@ -7524,30 +7663,30 @@
       <c r="AS13" s="1"/>
       <c r="AT13" s="1"/>
     </row>
-    <row r="14" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16" t="b">
@@ -7595,10 +7734,10 @@
       <c r="AS15" s="1"/>
       <c r="AT15" s="1"/>
     </row>
-    <row r="16" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -7606,180 +7745,180 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>13</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>14</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>15</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D19" s="69"/>
       <c r="E19" s="70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>16</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>17</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>20</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>21</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>22</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
         <v>23</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:46" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
         <v>24</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16" t="b">
@@ -7827,15 +7966,15 @@
       <c r="AS28" s="1"/>
       <c r="AT28" s="1"/>
     </row>
-    <row r="29" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>25</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="b">
@@ -7883,40 +8022,40 @@
       <c r="AS29" s="1"/>
       <c r="AT29" s="1"/>
     </row>
-    <row r="30" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
         <v>26</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>27</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -7924,92 +8063,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
         <v>27</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
         <v>28</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
         <v>29</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E35" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
         <v>30</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
         <v>31</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:46" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
         <v>32</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="16" t="b">
@@ -8057,40 +8196,40 @@
       <c r="AS38" s="30"/>
       <c r="AT38" s="30"/>
     </row>
-    <row r="39" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
         <v>33</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <v>34</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -8098,15 +8237,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="16" t="b">
@@ -8154,42 +8293,42 @@
       <c r="AS42" s="30"/>
       <c r="AT42" s="30"/>
     </row>
-    <row r="43" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <v>36</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
         <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E44" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -8197,62 +8336,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
         <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
         <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:46" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
         <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E48" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
         <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="16" t="b">
@@ -8300,42 +8439,42 @@
       <c r="AS49" s="1"/>
       <c r="AT49" s="1"/>
     </row>
-    <row r="50" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
         <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E50" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -8343,96 +8482,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
         <v>44</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E53" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <v>45</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:46" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
         <v>46</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E55" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="26">
         <v>47</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E56" s="28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A57" s="26">
         <v>48</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A58" s="26">
         <v>49</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="28" t="b">
@@ -8463,189 +8602,189 @@
       <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="66" style="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="36" customWidth="1"/>
     <col min="3" max="3" width="27" style="30" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="30" customWidth="1"/>
     <col min="5" max="5" width="20" style="30" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="30"/>
+    <col min="6" max="6" width="9.33203125" style="30"/>
     <col min="7" max="7" width="45" style="30" customWidth="1"/>
-    <col min="8" max="14" width="9.28515625" style="30"/>
-    <col min="15" max="15" width="70.140625" style="30" customWidth="1"/>
-    <col min="16" max="16384" width="9.28515625" style="30"/>
+    <col min="8" max="14" width="9.33203125" style="30"/>
+    <col min="15" max="15" width="70.109375" style="30" customWidth="1"/>
+    <col min="16" max="16384" width="9.33203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="49"/>
       <c r="B1" s="42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="E2" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="C3" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="D3" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="B4" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="C4" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="5" spans="1:8" ht="306" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="E3" s="39"/>
-    </row>
-    <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="B5" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="C4" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="E4" s="39"/>
-    </row>
-    <row r="5" spans="1:8" ht="318.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="D5" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:8" ht="108" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>281</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B6" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5" s="39"/>
-    </row>
-    <row r="6" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="D6" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="E6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
         <v>285</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="B7" s="34" t="s">
         <v>286</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="C7" s="35" t="s">
         <v>287</v>
-      </c>
-      <c r="E6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>290</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="40" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="D8" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="B9" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="C9" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>295</v>
       </c>
-      <c r="E8" s="39"/>
-    </row>
-    <row r="9" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B10" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>295</v>
-      </c>
-      <c r="E9" s="39" t="s">
+      <c r="C10" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="E10" s="39" t="s">
         <v>299</v>
       </c>
-      <c r="B10" s="34" t="s">
+    </row>
+    <row r="11" spans="1:8" ht="108" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" s="34" t="s">
+      <c r="B11" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="C11" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>305</v>
-      </c>
       <c r="E11" s="39"/>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -8653,352 +8792,352 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="34" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A15" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>309</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>295</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>312</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="E16" s="39" t="s">
         <v>313</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>316</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
     </row>
-    <row r="17" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="234" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="B17" s="34" t="s">
+    </row>
+    <row r="18" spans="1:15" ht="234" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
         <v>318</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D17" s="34" t="s">
+      <c r="B18" s="34" t="s">
         <v>319</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="C18" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="E18" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="B18" s="34" t="s">
+    </row>
+    <row r="19" spans="1:15" ht="234" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="C18" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D18" s="34" t="s">
+      <c r="B19" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="C19" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="262.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="E19" s="39" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="108" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B20" s="73" t="s">
         <v>326</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D19" s="34" t="s">
+      <c r="C20" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="108" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="B21" s="74" t="s">
         <v>328</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="C21" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>287</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
+      <c r="D21" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="E21" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="B22" s="73" t="s">
         <v>332</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="C22" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>287</v>
-      </c>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="D22" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="E22" s="39"/>
+    </row>
+    <row r="23" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="B23" s="73" t="s">
         <v>336</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="C23" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="E22" s="39"/>
-    </row>
-    <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="D23" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:15" ht="36" x14ac:dyDescent="0.3">
+      <c r="A24" s="38" t="s">
         <v>339</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="B24" s="73" t="s">
         <v>340</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="C24" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="D24" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E24" s="39"/>
+    </row>
+    <row r="25" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B25" s="73" t="s">
         <v>343</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C25" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="1:15" ht="54" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="D24" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
+      <c r="B26" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="C26" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>340</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E25" s="39"/>
-    </row>
-    <row r="26" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="D26" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E26" s="39"/>
+    </row>
+    <row r="27" spans="1:15" ht="162" x14ac:dyDescent="0.3">
+      <c r="A27" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B27" s="73" t="s">
         <v>348</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C27" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="D26" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E26" s="39"/>
-    </row>
-    <row r="27" spans="1:15" ht="168.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="D27" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="E27" s="39" t="s">
         <v>351</v>
       </c>
-      <c r="C27" s="34" t="s">
+    </row>
+    <row r="28" spans="1:15" ht="108" x14ac:dyDescent="0.3">
+      <c r="A28" s="38" t="s">
         <v>352</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="B28" s="73" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>353</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="D28" s="34" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+      <c r="E28" s="39" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="235.2" x14ac:dyDescent="0.65">
+      <c r="A29" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B29" s="73" t="s">
+        <v>348</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="E29" s="39" t="s">
         <v>351</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>356</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>357</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="236.25" x14ac:dyDescent="0.5">
-      <c r="A29" s="38" t="s">
+      <c r="O29" s="72" t="s">
         <v>358</v>
       </c>
-      <c r="B29" s="73" t="s">
-        <v>351</v>
-      </c>
-      <c r="C29" s="34" t="s">
+    </row>
+    <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="38" t="s">
         <v>359</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="B30" s="73" t="s">
+        <v>348</v>
+      </c>
+      <c r="C30" s="34" t="s">
         <v>360</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>354</v>
-      </c>
-      <c r="O29" s="72" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="B30" s="73" t="s">
-        <v>351</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>363</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="39" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="75"/>
     </row>
-    <row r="32" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="39" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.3">
+      <c r="A33" s="52" t="s">
+        <v>365</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="C33" s="41" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="52" t="s">
-        <v>368</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>370</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="39" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="C34" s="41" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
-        <v>371</v>
-      </c>
-      <c r="B34" s="41" t="s">
+      <c r="D34" s="34" t="s">
         <v>369</v>
       </c>
-      <c r="C34" s="41" t="s">
-        <v>370</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>372</v>
-      </c>
       <c r="E34" s="39" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="37" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="37" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add bin folder which currently has the prototype Jar files in them. bin = binary
</commit_message>
<xml_diff>
--- a/BLib_MindMap.xlsx
+++ b/BLib_MindMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Documents/Degree/5th Semester/BLib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF139C44-6C85-4640-984A-E82DF604FF22}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401728EE-A647-4A41-AAB2-38A142B38971}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="11220" yWindow="315" windowWidth="17280" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="2" r:id="rId1"/>
@@ -100,6 +100,13 @@
 Note: This file and UML diagrams are passed using the git repository.</t>
   </si>
   <si>
+    <t>ממשק אדם-מחשב מטלה 2</t>
+  </si>
+  <si>
+    <t>סדנה בתאריך 13/1/24
+בשעה: 13:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team Roles </t>
   </si>
   <si>
@@ -112,6 +119,12 @@
     <t>מטלה 2 שיטות (ממורקר)</t>
   </si>
   <si>
+    <t>חלוקת עבודה (לשונית Task2 - Engineering Methods)
+תאריך הגנה: 25/12/24 בכיתה M306
+הגשת אב טיפוס: 24/12/24 ב8:30
+הגשת שאר החלקים: 27/12/24 ב-16:00</t>
+  </si>
+  <si>
     <t>Meeting Schedule</t>
   </si>
   <si>
@@ -176,6 +189,12 @@
   </si>
   <si>
     <t>זוג מבצע</t>
+  </si>
+  <si>
+    <t>מי עשה בקרה?</t>
+  </si>
+  <si>
+    <t>עבר בקרה?</t>
   </si>
   <si>
     <t>ניקוד במטלה</t>
@@ -199,6 +218,9 @@
 </t>
   </si>
   <si>
+    <t>יניב + אלמוג</t>
+  </si>
+  <si>
     <t>* לפי הערה לשים לב: System לא נמצאת באף אחת מהדיאגרמות בפני עצמה</t>
   </si>
   <si>
@@ -214,6 +236,9 @@
   <si>
     <t>בניית Activity diagram עם Swimlanes.
 * דיאגרמה שנייה הל-"יצירת וצפיית בדו"ח סטטוס מנויים"</t>
+  </si>
+  <si>
+    <t>יובל + ליאור</t>
   </si>
   <si>
     <t xml:space="preserve">UML Diagrams </t>
@@ -249,6 +274,9 @@
     </r>
   </si>
   <si>
+    <t>ברגע שמסיימים עם ה-Sequence עוברים ל-Class</t>
+  </si>
+  <si>
     <t>ToDoList</t>
   </si>
   <si>
@@ -283,6 +311,12 @@
   </si>
   <si>
     <t>יש לכלול תיאור ארכיטקטורת התוכנה באמצעות Diagram Package. o במידת הצורך – השלמה עצמית של לימוד הנושא ב עזרת Google: לחפש: guidelines diagram Package, ולהשתמש בהגדרות והדוגמאות ב- .Lucidchart-ב או Visual Paradigm במטלה 3 תוערך איכות מודל זה מול מימוש ה- Packages בקוד והתיעוד שלהם .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">רון </t>
+  </si>
+  <si>
+    <t>יובל</t>
   </si>
   <si>
     <t>חלק 2: אב טיפוס  (25 נקודות)</t>
@@ -335,6 +369,9 @@
     <t>בנוסף יש להגיש בקובץ נפרד את ה-BACKLOG SPRINT עבור הספרינט השני )בין הגשה ראשונה לשנייה(. )כלומר יש להגיש את רשימת המשימות שתכננתם לביצוע בשלב הבנייה של הפרויקט: Log Product).</t>
   </si>
   <si>
+    <t>רון</t>
+  </si>
+  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -435,6 +472,21 @@
   </si>
   <si>
     <t>עבודה על גיט בחצי צוות</t>
+  </si>
+  <si>
+    <t>מפגש סדנה עם ג'וליה בנוגע למטלה 1 של ממשק אדם - מחשב + מפגש תיקון על המטלה</t>
+  </si>
+  <si>
+    <t>התחלת עבודה על מטלה 2 - שיטות הנדסיות, התחלת עבודה על UML</t>
+  </si>
+  <si>
+    <t>המשך עבודה על מטלה 2 של שיטות, המשך UML, התחלת בקרה על המטלה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סיום Sequence  ו- Activity </t>
+  </si>
+  <si>
+    <t>ביצוע בקרה על ה-UML השונים</t>
   </si>
   <si>
     <t>Category</t>
@@ -3713,56 +3765,6 @@
   </si>
   <si>
     <t>ENTER MORE INFORMATION AS NEEDED</t>
-  </si>
-  <si>
-    <t>יובל</t>
-  </si>
-  <si>
-    <t>יניב + אלמוג</t>
-  </si>
-  <si>
-    <t>יובל + ליאור</t>
-  </si>
-  <si>
-    <t xml:space="preserve">רון </t>
-  </si>
-  <si>
-    <t>ברגע שמסיימים עם ה-Sequence עוברים ל-Class</t>
-  </si>
-  <si>
-    <t>רון</t>
-  </si>
-  <si>
-    <t>עבר בקרה?</t>
-  </si>
-  <si>
-    <t>מי עשה בקרה?</t>
-  </si>
-  <si>
-    <t>מפגש סדנה עם ג'וליה בנוגע למטלה 1 של ממשק אדם - מחשב + מפגש תיקון על המטלה</t>
-  </si>
-  <si>
-    <t>התחלת עבודה על מטלה 2 - שיטות הנדסיות, התחלת עבודה על UML</t>
-  </si>
-  <si>
-    <t>המשך עבודה על מטלה 2 של שיטות, המשך UML, התחלת בקרה על המטלה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">סיום Sequence  ו- Activity </t>
-  </si>
-  <si>
-    <t>ביצוע בקרה על ה-UML השונים</t>
-  </si>
-  <si>
-    <t>ממשק אדם-מחשב מטלה 2</t>
-  </si>
-  <si>
-    <t>סדנה בתאריך 13/1/24
-בשעה: 13:30</t>
-  </si>
-  <si>
-    <t>חלוקת עבודה (לשונית Task2 - Engineering Methods)
-תאריך הגנה: 25/12/24 בכיתה M306</t>
   </si>
 </sst>
 </file>
@@ -5594,7 +5596,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5617,7 +5619,7 @@
       </c>
       <c r="G1" s="65">
         <f ca="1">TODAY()</f>
-        <v>45643</v>
+        <v>45649</v>
       </c>
       <c r="I1" s="61"/>
     </row>
@@ -5661,55 +5663,55 @@
         <v>0</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>383</v>
+        <v>12</v>
       </c>
       <c r="G3" s="61">
         <v>45658</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>384</v>
+        <v>13</v>
       </c>
       <c r="I3" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="58" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="61">
         <v>45650</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>385</v>
+        <v>18</v>
       </c>
       <c r="I4" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="58" t="b">
         <v>0</v>
@@ -5720,13 +5722,13 @@
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" s="58" t="b">
         <v>0</v>
@@ -5736,13 +5738,13 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E7" s="58" t="b">
         <v>0</v>
@@ -5752,13 +5754,13 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E8" s="58" t="b">
         <v>0</v>
@@ -5788,7 +5790,7 @@
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C11" s="46"/>
       <c r="E11" s="58" t="b">
@@ -5800,10 +5802,10 @@
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" s="58" t="b">
         <v>0</v>
@@ -5813,13 +5815,13 @@
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E13" s="58" t="b">
         <v>0</v>
@@ -5830,13 +5832,13 @@
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E14" s="58" t="b">
         <v>0</v>
@@ -5846,10 +5848,10 @@
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E15" s="58" t="b">
         <v>0</v>
@@ -6028,42 +6030,42 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>377</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>376</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H1" s="84" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="84"/>
       <c r="J1" s="81" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K1" s="82" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="83"/>
       <c r="C2" s="80" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -6072,21 +6074,21 @@
       <c r="H2" s="87"/>
       <c r="I2" s="84"/>
       <c r="J2" s="81" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>371</v>
+        <v>49</v>
       </c>
       <c r="D3" s="88" t="b">
         <v>0</v>
@@ -6099,25 +6101,25 @@
         <v>18</v>
       </c>
       <c r="H3" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I3" s="84"/>
       <c r="J3" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B4" s="85" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>372</v>
+        <v>55</v>
       </c>
       <c r="D4" s="88" t="b">
         <v>1</v>
@@ -6128,26 +6130,26 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>374</v>
+        <v>60</v>
       </c>
       <c r="D5" s="88" t="b">
         <v>0</v>
@@ -6160,25 +6162,25 @@
         <v>30</v>
       </c>
       <c r="H5" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="29" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>371</v>
+        <v>49</v>
       </c>
       <c r="D6" s="88" t="b">
         <v>0</v>
@@ -6191,25 +6193,25 @@
         <v>12</v>
       </c>
       <c r="H6" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="66" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B7" s="85" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>372</v>
+        <v>55</v>
       </c>
       <c r="D7" s="88" t="b">
         <v>1</v>
@@ -6220,29 +6222,29 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I7" s="84"/>
       <c r="J7" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B8" s="85" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>373</v>
+        <v>72</v>
       </c>
       <c r="D8" s="88" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>370</v>
+        <v>73</v>
       </c>
       <c r="F8" s="88" t="b">
         <v>0</v>
@@ -6251,7 +6253,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I8" s="84"/>
     </row>
@@ -6259,7 +6261,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="83"/>
       <c r="C9" s="80" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -6269,18 +6271,18 @@
       <c r="I9" s="84"/>
       <c r="J9" s="90">
         <f ca="1">'Important Information'!I4</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K9" s="89" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B10" s="85" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="88" t="b">
@@ -6298,10 +6300,10 @@
     </row>
     <row r="11" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B11" s="85" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="88" t="b">
@@ -6318,7 +6320,7 @@
     <row r="12" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="85" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="88" t="b">
@@ -6334,10 +6336,10 @@
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B13" s="85" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="88" t="b">
@@ -6353,10 +6355,10 @@
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B14" s="85" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="88" t="b">
@@ -6368,7 +6370,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="85" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="I14" s="85"/>
     </row>
@@ -6376,7 +6378,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="83"/>
       <c r="C15" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6387,13 +6389,13 @@
     </row>
     <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B16" s="85" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>370</v>
+        <v>73</v>
       </c>
       <c r="D16" s="88" t="b">
         <v>1</v>
@@ -6410,19 +6412,19 @@
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B17" s="85" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>375</v>
+        <v>89</v>
       </c>
       <c r="D17" s="88" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>370</v>
+        <v>73</v>
       </c>
       <c r="F17" s="88" t="b">
         <v>0</v>
@@ -6489,101 +6491,101 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="77" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="77" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="77" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="77" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="77" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="77" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -6611,10 +6613,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -6625,7 +6627,7 @@
         <v>45617</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -6634,7 +6636,7 @@
         <v>45619</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -6643,7 +6645,7 @@
         <v>45622</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -6652,7 +6654,7 @@
         <v>45624</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -6661,7 +6663,7 @@
         <v>45625</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -6670,7 +6672,7 @@
         <v>45628</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -6679,7 +6681,7 @@
         <v>45630</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -6688,7 +6690,7 @@
         <v>45635</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>378</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -6697,7 +6699,7 @@
         <v>45636</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>379</v>
+        <v>124</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -6706,7 +6708,7 @@
         <v>45638</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>380</v>
+        <v>125</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -6715,7 +6717,7 @@
         <v>45639</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>381</v>
+        <v>126</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -6724,7 +6726,7 @@
         <v>45640</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>382</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -6907,420 +6909,420 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C29" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C32" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C36" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -7352,26 +7354,26 @@
   <sheetData>
     <row r="1" spans="1:46" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:46" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -7425,10 +7427,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="b">
@@ -7440,10 +7442,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="b">
@@ -7455,10 +7457,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16" t="b">
@@ -7470,10 +7472,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="b">
@@ -7485,10 +7487,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="b">
@@ -7500,10 +7502,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="b">
@@ -7515,10 +7517,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16" t="b">
@@ -7569,7 +7571,7 @@
     <row r="10" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7582,10 +7584,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="20"/>
@@ -7595,10 +7597,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="b">
@@ -7651,10 +7653,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16" t="b">
@@ -7707,10 +7709,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="b">
@@ -7722,10 +7724,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16" t="b">
@@ -7776,7 +7778,7 @@
     <row r="16" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -7789,10 +7791,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16" t="b">
@@ -7804,10 +7806,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>219</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>203</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="b">
@@ -7819,10 +7821,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D19" s="69"/>
       <c r="E19" s="70" t="b">
@@ -7834,10 +7836,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16" t="b">
@@ -7849,10 +7851,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16" t="b">
@@ -7864,10 +7866,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="b">
@@ -7879,10 +7881,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16" t="b">
@@ -7894,10 +7896,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="b">
@@ -7909,10 +7911,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="b">
@@ -7924,10 +7926,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16" t="b">
@@ -7939,10 +7941,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16" t="b">
@@ -7954,10 +7956,10 @@
         <v>24</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16" t="b">
@@ -8010,10 +8012,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="b">
@@ -8066,10 +8068,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16" t="b">
@@ -8081,10 +8083,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16" t="b">
@@ -8094,7 +8096,7 @@
     <row r="32" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -8107,10 +8109,10 @@
         <v>27</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="16" t="b">
@@ -8122,10 +8124,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="16" t="b">
@@ -8137,13 +8139,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="E35" s="16" t="b">
         <v>0</v>
@@ -8154,10 +8156,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16" t="b">
@@ -8169,10 +8171,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="16" t="b">
@@ -8184,10 +8186,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="16" t="b">
@@ -8240,10 +8242,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="16" t="b">
@@ -8255,10 +8257,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16" t="b">
@@ -8268,7 +8270,7 @@
     <row r="41" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -8281,10 +8283,10 @@
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="16" t="b">
@@ -8337,10 +8339,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="16" t="b">
@@ -8352,13 +8354,13 @@
         <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="E44" s="16" t="b">
         <v>0</v>
@@ -8367,7 +8369,7 @@
     <row r="45" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -8380,10 +8382,10 @@
         <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16" t="b">
@@ -8395,10 +8397,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="16" t="b">
@@ -8410,13 +8412,13 @@
         <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="E48" s="16" t="b">
         <v>0</v>
@@ -8427,10 +8429,10 @@
         <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="16" t="b">
@@ -8483,13 +8485,13 @@
         <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="E50" s="16" t="b">
         <v>0</v>
@@ -8500,10 +8502,10 @@
         <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16" t="b">
@@ -8513,7 +8515,7 @@
     <row r="52" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -8526,13 +8528,13 @@
         <v>44</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="E53" s="16" t="b">
         <v>0</v>
@@ -8543,10 +8545,10 @@
         <v>45</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16" t="b">
@@ -8558,13 +8560,13 @@
         <v>46</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="E55" s="16" t="b">
         <v>0</v>
@@ -8575,13 +8577,13 @@
         <v>47</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="E56" s="28" t="b">
         <v>0</v>
@@ -8592,10 +8594,10 @@
         <v>48</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="28" t="b">
@@ -8607,10 +8609,10 @@
         <v>49</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="28" t="b">
@@ -8658,7 +8660,7 @@
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
       <c r="B1" s="42" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -8666,164 +8668,164 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:8" ht="318.75" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="40" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="E11" s="39"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -8833,14 +8835,14 @@
     </row>
     <row r="14" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="34" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="36"/>
@@ -8849,19 +8851,19 @@
     </row>
     <row r="15" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="C15" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>291</v>
-      </c>
       <c r="E15" s="39" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -8869,19 +8871,19 @@
     </row>
     <row r="16" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="E16" s="39" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -8889,238 +8891,238 @@
     </row>
     <row r="17" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="262.5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B19" s="73" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>326</v>
+        <v>342</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>330</v>
+        <v>346</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>335</v>
+        <v>351</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>340</v>
+        <v>356</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>342</v>
+        <v>358</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
       <c r="B26" s="73" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
       <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:15" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>348</v>
+        <v>364</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="236.25" x14ac:dyDescent="0.5">
       <c r="A29" s="38" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
       <c r="O29" s="72" t="s">
-        <v>357</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
-        <v>358</v>
+        <v>374</v>
       </c>
       <c r="B30" s="73" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>359</v>
+        <v>375</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="39" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -9128,55 +9130,55 @@
     </row>
     <row r="32" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
-        <v>360</v>
+        <v>376</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>361</v>
+        <v>377</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>362</v>
+        <v>378</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="39" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>366</v>
+        <v>382</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="39" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>366</v>
+        <v>382</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>368</v>
+        <v>384</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="37" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>369</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete Prtotype - old version
</commit_message>
<xml_diff>
--- a/BLib_MindMap.xlsx
+++ b/BLib_MindMap.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Documents/Degree/5th Semester/BLib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401728EE-A647-4A41-AAB2-38A142B38971}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6CC2DE1-0943-484A-BA39-46E1F8E9FE62}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="2" r:id="rId1"/>
-    <sheet name="Task2 - Engineering Methods" sheetId="8" r:id="rId2"/>
-    <sheet name="Team Roles " sheetId="7" r:id="rId3"/>
-    <sheet name="Meeting Schedule" sheetId="5" r:id="rId4"/>
-    <sheet name="Code Standards" sheetId="4" r:id="rId5"/>
-    <sheet name="Requirements" sheetId="1" r:id="rId6"/>
-    <sheet name="Acceptance Testing" sheetId="3" r:id="rId7"/>
+    <sheet name="Task2 - Man-Machine Interface" sheetId="9" r:id="rId2"/>
+    <sheet name="Task2 - Engineering Methods" sheetId="8" r:id="rId3"/>
+    <sheet name="Team Roles " sheetId="7" r:id="rId4"/>
+    <sheet name="Meeting Schedule" sheetId="5" r:id="rId5"/>
+    <sheet name="Code Standards" sheetId="4" r:id="rId6"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId7"/>
+    <sheet name="Acceptance Testing" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,6 +45,25 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={6E29D5BF-9127-491B-921F-EA8660ABC542}</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{6E29D5BF-9127-491B-921F-EA8660ABC542}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    תכניס קישור ל-FIGMA
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={F65DB051-A65E-44A4-A28C-7BA965ADD77C}</author>
   </authors>
   <commentList>
@@ -61,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="417">
   <si>
     <t>Group No. 5</t>
   </si>
@@ -117,12 +137,6 @@
   </si>
   <si>
     <t>מטלה 2 שיטות (ממורקר)</t>
-  </si>
-  <si>
-    <t>חלוקת עבודה (לשונית Task2 - Engineering Methods)
-תאריך הגנה: 25/12/24 בכיתה M306
-הגשת אב טיפוס: 24/12/24 ב8:30
-הגשת שאר החלקים: 27/12/24 ב-16:00</t>
   </si>
   <si>
     <t>Meeting Schedule</t>
@@ -3766,12 +3780,116 @@
   <si>
     <t>ENTER MORE INFORMATION AS NEEDED</t>
   </si>
+  <si>
+    <t>שאר החלקים בשיטות</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>חלוקת עבודה (לשונית Task2 - Engineering Methods)
+תאריך הגנה: 25/12/24 בכיתה M306
+בשעה 10:30
+הגשת אב טיפוס: 24/12/24 ב8:30
+הגשת שאר החלקים: 27/12/24 ב-16:00</t>
+  </si>
+  <si>
+    <t>נשאר להחליט האם לפצל את הקובץ לספרינט 2 בלבד או שלא.</t>
+  </si>
+  <si>
+    <t>נשלח</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>סיפור מטלה 1</t>
+  </si>
+  <si>
+    <t>מטלה 1 - ראיונות והסקת מסקנות</t>
+  </si>
+  <si>
+    <t>מטלה 2 - HTL + אב טיפוס</t>
+  </si>
+  <si>
+    <t>המשך עבודה על ה-Prototype</t>
+  </si>
+  <si>
+    <t>סיום עבודה על מטלה 2 של שיטות הנדסיות + התחלת עבודה על ממשק אדם-מחשב מטלה 2</t>
+  </si>
+  <si>
+    <t>קישורים</t>
+  </si>
+  <si>
+    <t>HTL</t>
+  </si>
+  <si>
+    <t>Low Level Prototype</t>
+  </si>
+  <si>
+    <t>מצגת HTL ממורקרת</t>
+  </si>
+  <si>
+    <t>מצגת LOW LEVEL PROTOTYPE ממורקרת</t>
+  </si>
+  <si>
+    <t>הערות UML:</t>
+  </si>
+  <si>
+    <t>מה לעשות?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תרשים ACTIVITY השאלת ספר </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ב-Class דיאגרם, חיבור לתיקיה של הJDBC </t>
+  </si>
+  <si>
+    <t>נשאיר אץ האובייקטים -&gt; בחיבור גנרי לתיקייה.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ב-Class היא אמרה שהיא רוצה לראות 2 דברים אבסטרקטיים ו-2 דברים </t>
+  </si>
+  <si>
+    <t>להכניס ABSTRACT SERVER ו-SERVER UI
+להכניס ABSTRACT CLIENT ו-CLIENT UI</t>
+  </si>
+  <si>
+    <t>צריך לפצל ל-3 דיאגרמות שונות
+תהליך השאלה
+תהליך החזרה
+תהליך הארכה</t>
+  </si>
+  <si>
+    <t>האם לחבר את הJAVAFX רק לDB?</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>האם SERVER SERVICE יורש ממישהו? יכול להיות שחסרים CLASS-ים</t>
+  </si>
+  <si>
+    <t>לעשות בדיקה בקוד ולגזור מסקנות</t>
+  </si>
+  <si>
+    <t>להוסיף את ECHO SERVER שמחובר לJAVAFX</t>
+  </si>
+  <si>
+    <t>להכניס את ה-Class של ConnectToDB</t>
+  </si>
+  <si>
+    <t>לעשות התאמה יסודית בין האבטיפוס לתרשים מחלקות</t>
+  </si>
+  <si>
+    <t>! השוואה אחרונה על הכל ושגר ושכח</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3906,6 +4024,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="8">
@@ -4076,7 +4199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4394,12 +4517,84 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4504,6 +4699,40 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5176,90 +5405,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A2:C17" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="74" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="95" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
-  <autoFilter ref="E2:I15" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="65"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:H17" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
-  <autoFilter ref="A1:H17" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{6F08DEB8-9412-4A60-827F-650CE5DE012A}" name="מי עשה בקרה?" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{0B213265-848E-42AD-BB24-FACA108AE82B}" name="עבר בקרה?" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{C212956F-6717-4ACE-9560-C2C858E916CC}" name="ניקוד במטלה" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{4BAEA3F5-7A0E-45FC-BD15-78D20A6CE5AF}" name="הערות" dataDxfId="55"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="J3:K7" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="J3:K7" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9D0FE680-0194-44E8-8173-C409E67F91A6}" name="קישור" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{4D3F5656-E6FB-49EB-ACFD-772E84A9C306}" name="הסבר" dataDxfId="51"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="A1:E7" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7DD096F3-29E7-44B9-8E03-74AE8B0EFB58}" name="Full Name" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{86460309-D719-48D5-BE5A-FED925E8C505}" name="תפקיד 1 - שיטות" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{47A50531-CD06-43C3-AF93-5FE6CE915387}" name="תפקיד 2 - שיטות" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{9327F458-CD94-484D-95E0-7A5C295651CA}" name="תפקיד 1 - ממשק אדם - מחשב" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{875991B2-2D2B-439E-AAE3-9B4D6238D1C7}" name="Comments" dataDxfId="44"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C41" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:C41" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="39"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36">
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A1:C38" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{250D87B3-0E0E-41F7-BADF-53EC76930D5E}" name="Specification"/>
     <tableColumn id="3" xr3:uid="{53542E77-0500-4A50-A0B6-226ADBB40CAE}" name="Details"/>
   </tableColumns>
@@ -5267,29 +5428,131 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:E58" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:E58" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="A2:E34" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="36"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
+  <autoFilter ref="E2:I15" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="86"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{987D062A-F148-4472-B909-8204292FB429}" name="Table9" displayName="Table9" ref="A1:A6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:A6" xr:uid="{987D062A-F148-4472-B909-8204292FB429}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{AE01AEED-CFF1-4414-9EAA-6174383BCA7C}" name="Links" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C95D32FB-859B-4209-80FF-339F84A4F767}" name="Table10" displayName="Table10" ref="C1:E3" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="C1:E3" xr:uid="{C95D32FB-859B-4209-80FF-339F84A4F767}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EEF69765-8BBA-402D-ADC3-9CDFD9D37FA1}" name="משימה" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{ED6C2DC2-A67D-4080-90BF-59C9DD16DCC2}" name="בוצע?" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{718425F0-840A-4FA7-A37E-5EB58D90FD0F}" name="קישורים" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:H17" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
+  <autoFilter ref="A1:H17" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{6F08DEB8-9412-4A60-827F-650CE5DE012A}" name="מי עשה בקרה?" dataDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{0B213265-848E-42AD-BB24-FACA108AE82B}" name="עבר בקרה?" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{C212956F-6717-4ACE-9560-C2C858E916CC}" name="ניקוד במטלה" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{4BAEA3F5-7A0E-45FC-BD15-78D20A6CE5AF}" name="הערות" dataDxfId="76"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="J3:K7" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+  <autoFilter ref="J3:K7" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9D0FE680-0194-44E8-8173-C409E67F91A6}" name="קישור" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{4D3F5656-E6FB-49EB-ACFD-772E84A9C306}" name="הסבר" dataDxfId="72"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C7AC7C6D-F385-46C1-AF38-CDA1CFB529BE}" name="Table11" displayName="Table11" ref="A19:C30" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A19:C30" xr:uid="{C7AC7C6D-F385-46C1-AF38-CDA1CFB529BE}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{57D5C4F4-64FD-4EFD-808E-E0801EF70843}" name="הערות UML:" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F806FB25-CBE9-4A56-911B-78A294B244BB}" name="מה לעשות?" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6769BA36-EFA5-494A-86DC-C52F5A3CBC10}" name="בוצע?" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A1:E7" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7DD096F3-29E7-44B9-8E03-74AE8B0EFB58}" name="Full Name" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{86460309-D719-48D5-BE5A-FED925E8C505}" name="תפקיד 1 - שיטות" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{47A50531-CD06-43C3-AF93-5FE6CE915387}" name="תפקיד 2 - שיטות" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{9327F458-CD94-484D-95E0-7A5C295651CA}" name="תפקיד 1 - ממשק אדם - מחשב" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{875991B2-2D2B-439E-AAE3-9B4D6238D1C7}" name="Comments" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A2:E34" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C41" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+  <autoFilter ref="A1:C41" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5582,6 +5845,15 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E3" dT="2024-12-24T15:44:35.95" personId="{0020C943-DF8D-440E-A473-11A712E33C2F}" id="{6E29D5BF-9127-491B-921F-EA8660ABC542}">
+    <text xml:space="preserve">תכניס קישור ל-FIGMA
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="K2" dT="2024-11-27T06:56:30.52" personId="{0020C943-DF8D-440E-A473-11A712E33C2F}" id="{F65DB051-A65E-44A4-A28C-7BA965ADD77C}">
     <text xml:space="preserve">משוך נתונים על החברי צוות ותפקידים
 </text>
@@ -5593,10 +5865,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E429A24-44E4-45FF-AD25-4F9463F77043}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5619,7 +5891,7 @@
       </c>
       <c r="G1" s="65">
         <f ca="1">TODAY()</f>
-        <v>45649</v>
+        <v>45650</v>
       </c>
       <c r="I1" s="61"/>
     </row>
@@ -5673,10 +5945,10 @@
       </c>
       <c r="I3" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>14</v>
       </c>
@@ -5696,39 +5968,49 @@
         <v>45650</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>18</v>
+        <v>387</v>
       </c>
       <c r="I4" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="58" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="61"/>
-      <c r="I5" s="64"/>
+      <c r="F5" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="G5" s="61">
+        <v>45653</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I5" s="64">
+        <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="58" t="b">
         <v>0</v>
@@ -5738,13 +6020,13 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="58" t="b">
         <v>0</v>
@@ -5754,13 +6036,13 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="58" t="b">
         <v>0</v>
@@ -5790,7 +6072,7 @@
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="46"/>
       <c r="E11" s="58" t="b">
@@ -5802,10 +6084,10 @@
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="58" t="b">
         <v>0</v>
@@ -5815,13 +6097,13 @@
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E13" s="58" t="b">
         <v>0</v>
@@ -5832,13 +6114,13 @@
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="58" t="b">
         <v>0</v>
@@ -5848,10 +6130,10 @@
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E15" s="58" t="b">
         <v>0</v>
@@ -5952,15 +6234,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5999,22 +6281,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618B7F2F-AA11-49D6-A471-6DBFD27DE173}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="91" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="92" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" s="91" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="92" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="91"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="92" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="91"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="91"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="92" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" s="91"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="91"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="92" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="91"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="91"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="91"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="91"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="91"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="91"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{E32A146A-B98D-4D37-9498-F6407D29D63C}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4B2BBD88-94E6-4C36-A578-8CC45EEDF9F1}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{A3B230C3-1628-491A-8BFF-896CF90CF594}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{F46D9DCC-8850-4F61-AD89-BC14EEA85B5A}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{26819A99-002C-4F36-BE38-7D9F1553F5C4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId6"/>
+  <tableParts count="2">
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41833F2A-0F74-46A8-96BA-249A656C284B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.28515625" style="85" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" style="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="78" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" style="78" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="78" customWidth="1"/>
     <col min="7" max="7" width="16" style="78" bestFit="1" customWidth="1"/>
@@ -6030,25 +6433,25 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H1" s="84" t="s">
         <v>7</v>
@@ -6058,14 +6461,14 @@
         <v>17</v>
       </c>
       <c r="K1" s="82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="83"/>
       <c r="C2" s="80" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -6074,21 +6477,21 @@
       <c r="H2" s="87"/>
       <c r="I2" s="84"/>
       <c r="J2" s="81" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="C3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="88" t="b">
         <v>0</v>
@@ -6101,25 +6504,25 @@
         <v>18</v>
       </c>
       <c r="H3" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" s="84"/>
       <c r="J3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="C4" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D4" s="88" t="b">
         <v>1</v>
@@ -6130,26 +6533,26 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="C5" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D5" s="88" t="b">
         <v>0</v>
@@ -6162,25 +6565,25 @@
         <v>30</v>
       </c>
       <c r="H5" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="85" t="s">
-        <v>64</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="88" t="b">
         <v>0</v>
@@ -6193,25 +6596,25 @@
         <v>12</v>
       </c>
       <c r="H6" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="85" t="s">
-        <v>68</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="88" t="b">
         <v>1</v>
@@ -6222,29 +6625,31 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="84"/>
-      <c r="J7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="2"/>
+      <c r="J7" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="60" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="C8" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D8" s="88" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="88" t="b">
         <v>0</v>
@@ -6253,7 +6658,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="84"/>
     </row>
@@ -6261,7 +6666,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="83"/>
       <c r="C9" s="80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -6271,18 +6676,18 @@
       <c r="I9" s="84"/>
       <c r="J9" s="90">
         <f ca="1">'Important Information'!I4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="85" t="s">
         <v>76</v>
-      </c>
-      <c r="B10" s="85" t="s">
-        <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="88" t="b">
@@ -6300,10 +6705,10 @@
     </row>
     <row r="11" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="85" t="s">
         <v>78</v>
-      </c>
-      <c r="B11" s="85" t="s">
-        <v>79</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="88" t="b">
@@ -6320,7 +6725,7 @@
     <row r="12" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="88" t="b">
@@ -6336,10 +6741,10 @@
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="85" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" s="85" t="s">
-        <v>82</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="88" t="b">
@@ -6355,10 +6760,10 @@
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="85" t="s">
         <v>83</v>
-      </c>
-      <c r="B14" s="85" t="s">
-        <v>84</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="88" t="b">
@@ -6370,7 +6775,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="85"/>
     </row>
@@ -6378,7 +6783,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="83"/>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -6389,20 +6794,20 @@
     </row>
     <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="85" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="88" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>10</v>
@@ -6410,30 +6815,32 @@
       <c r="H16" s="84"/>
       <c r="I16" s="84"/>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D17" s="88" t="b">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="84"/>
+      <c r="H17" s="87" t="s">
+        <v>388</v>
+      </c>
       <c r="I17" s="84"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -6443,16 +6850,320 @@
       <c r="H18" s="84"/>
       <c r="I18" s="84"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="79"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C20" s="88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C21" s="88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C22" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="78"/>
+      <c r="J22" s="86"/>
+      <c r="L22" s="79"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C23" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="78"/>
+      <c r="J23" s="86"/>
+      <c r="L23" s="79"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C24" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="78"/>
+      <c r="J24" s="86"/>
+      <c r="L24" s="79"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="78"/>
+      <c r="J25" s="86"/>
+      <c r="L25" s="79"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C26" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="78"/>
+      <c r="J26" s="86"/>
+      <c r="L26" s="79"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="78"/>
+      <c r="J27" s="86"/>
+      <c r="L27" s="79"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="78"/>
+      <c r="J28" s="86"/>
+      <c r="L28" s="79"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="78"/>
+      <c r="J29" s="86"/>
+      <c r="L29" s="79"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="88" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="78"/>
+      <c r="J30" s="86"/>
+      <c r="L30" s="79"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H31" s="78"/>
+      <c r="J31" s="86"/>
+      <c r="L31" s="79"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" s="78"/>
+      <c r="J32" s="86"/>
+      <c r="L32" s="79"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H33" s="78"/>
+      <c r="J33" s="86"/>
+      <c r="L33" s="79"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H34" s="78"/>
+      <c r="J34" s="86"/>
+      <c r="L34" s="79"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="H35" s="78"/>
+      <c r="J35" s="86"/>
+      <c r="L35" s="79"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="H36" s="78"/>
+      <c r="J36" s="86"/>
+      <c r="L36" s="79"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="H37" s="78"/>
+      <c r="J37" s="86"/>
+      <c r="L37" s="79"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="H38" s="78"/>
+      <c r="J38" s="86"/>
+      <c r="L38" s="79"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="H39" s="78"/>
+      <c r="J39" s="86"/>
+      <c r="L39" s="79"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="H40" s="78"/>
+      <c r="J40" s="86"/>
+      <c r="L40" s="79"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="H41" s="78"/>
+      <c r="J41" s="86"/>
+      <c r="L41" s="79"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="H42" s="78"/>
+      <c r="J42" s="86"/>
+      <c r="L42" s="79"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="H43" s="78"/>
+      <c r="J43" s="86"/>
+      <c r="L43" s="79"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="H44" s="78"/>
+      <c r="J44" s="86"/>
+      <c r="L44" s="79"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="H45" s="78"/>
+      <c r="J45" s="86"/>
+      <c r="L45" s="79"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="H46" s="78"/>
+      <c r="J46" s="86"/>
+      <c r="L46" s="79"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="H47" s="78"/>
+      <c r="J47" s="86"/>
+      <c r="L47" s="79"/>
     </row>
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
   <conditionalFormatting sqref="D3:D8 F3:F8 D10:D14 F10:F14 D16:D17 F16:F17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C30">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6464,19 +7175,20 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE753598-B63F-4BFF-A796-9131C2B9321B}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6491,101 +7203,101 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -6597,12 +7309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538DB23-0864-46D9-82F7-B6A0E6DA13F2}">
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6613,10 +7325,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -6627,7 +7339,7 @@
         <v>45617</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -6636,7 +7348,7 @@
         <v>45619</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -6645,7 +7357,7 @@
         <v>45622</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -6654,7 +7366,7 @@
         <v>45624</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -6663,7 +7375,7 @@
         <v>45625</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -6672,7 +7384,7 @@
         <v>45628</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -6681,7 +7393,7 @@
         <v>45630</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -6690,7 +7402,7 @@
         <v>45635</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -6699,7 +7411,7 @@
         <v>45636</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -6708,7 +7420,7 @@
         <v>45638</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -6717,7 +7429,7 @@
         <v>45639</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -6726,7 +7438,7 @@
         <v>45640</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -6734,14 +7446,18 @@
       <c r="A14" s="76">
         <v>45643</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="76">
         <v>45650</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6892,7 +7608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0F8AA7-3D0F-4359-84F6-848A1B337549}">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -6909,420 +7625,420 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="C1" s="54" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" s="54" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
         <v>131</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>132</v>
-      </c>
-      <c r="C2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
         <v>134</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
         <v>136</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
         <v>138</v>
-      </c>
-      <c r="C5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" t="s">
         <v>140</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
         <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" t="s">
         <v>144</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>145</v>
-      </c>
-      <c r="C8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
         <v>147</v>
-      </c>
-      <c r="C9" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" t="s">
         <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" t="s">
         <v>151</v>
-      </c>
-      <c r="C11" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" t="s">
         <v>153</v>
-      </c>
-      <c r="C12" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
         <v>155</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>156</v>
-      </c>
-      <c r="C13" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" t="s">
         <v>158</v>
-      </c>
-      <c r="C14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" t="s">
         <v>160</v>
-      </c>
-      <c r="C15" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" t="s">
         <v>162</v>
-      </c>
-      <c r="C16" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" t="s">
         <v>164</v>
-      </c>
-      <c r="C17" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" t="s">
         <v>166</v>
-      </c>
-      <c r="C18" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
         <v>168</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>169</v>
-      </c>
-      <c r="C19" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
         <v>171</v>
-      </c>
-      <c r="C20" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" t="s">
         <v>173</v>
-      </c>
-      <c r="C21" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" t="s">
         <v>175</v>
-      </c>
-      <c r="B22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" t="s">
         <v>178</v>
-      </c>
-      <c r="C24" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
         <v>180</v>
-      </c>
-      <c r="C25" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
         <v>182</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>183</v>
-      </c>
-      <c r="C26" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" t="s">
         <v>185</v>
-      </c>
-      <c r="C27" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" t="s">
         <v>187</v>
-      </c>
-      <c r="C28" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" t="s">
         <v>189</v>
-      </c>
-      <c r="C29" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" t="s">
         <v>191</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>192</v>
-      </c>
-      <c r="C30" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" t="s">
         <v>194</v>
-      </c>
-      <c r="C31" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" t="s">
         <v>196</v>
-      </c>
-      <c r="C32" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" t="s">
         <v>198</v>
-      </c>
-      <c r="C33" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" t="s">
         <v>200</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>201</v>
-      </c>
-      <c r="C34" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" t="s">
         <v>203</v>
-      </c>
-      <c r="C35" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" t="s">
         <v>205</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>206</v>
-      </c>
-      <c r="C36" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B37" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" t="s">
         <v>208</v>
-      </c>
-      <c r="C37" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" t="s">
         <v>210</v>
-      </c>
-      <c r="C38" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -7333,7 +8049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT58"/>
   <sheetViews>
@@ -7354,26 +8070,26 @@
   <sheetData>
     <row r="1" spans="1:46" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:46" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -7427,10 +8143,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>218</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>219</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="b">
@@ -7442,10 +8158,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="b">
@@ -7457,10 +8173,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>221</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>222</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16" t="b">
@@ -7472,10 +8188,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="b">
@@ -7487,10 +8203,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="b">
@@ -7502,10 +8218,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="b">
@@ -7517,10 +8233,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16" t="b">
@@ -7571,7 +8287,7 @@
     <row r="10" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -7584,10 +8300,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="20"/>
@@ -7597,10 +8313,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="b">
@@ -7653,10 +8369,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16" t="b">
@@ -7709,10 +8425,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16" t="b">
@@ -7724,10 +8440,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16" t="b">
@@ -7778,7 +8494,7 @@
     <row r="16" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -7791,10 +8507,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16" t="b">
@@ -7806,10 +8522,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16" t="b">
@@ -7821,10 +8537,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" s="69"/>
       <c r="E19" s="70" t="b">
@@ -7836,10 +8552,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16" t="b">
@@ -7851,10 +8567,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16" t="b">
@@ -7866,10 +8582,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="b">
@@ -7881,10 +8597,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16" t="b">
@@ -7896,10 +8612,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16" t="b">
@@ -7911,10 +8627,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="b">
@@ -7926,10 +8642,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16" t="b">
@@ -7941,10 +8657,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16" t="b">
@@ -7956,10 +8672,10 @@
         <v>24</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16" t="b">
@@ -8012,10 +8728,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16" t="b">
@@ -8068,10 +8784,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16" t="b">
@@ -8083,10 +8799,10 @@
         <v>27</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16" t="b">
@@ -8096,7 +8812,7 @@
     <row r="32" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -8109,10 +8825,10 @@
         <v>27</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="16" t="b">
@@ -8124,10 +8840,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="16" t="b">
@@ -8139,13 +8855,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>253</v>
       </c>
       <c r="E35" s="16" t="b">
         <v>0</v>
@@ -8156,10 +8872,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16" t="b">
@@ -8171,10 +8887,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="16" t="b">
@@ -8186,10 +8902,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="16" t="b">
@@ -8242,10 +8958,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="16" t="b">
@@ -8257,10 +8973,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16" t="b">
@@ -8270,7 +8986,7 @@
     <row r="41" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -8283,10 +8999,10 @@
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="16" t="b">
@@ -8339,10 +9055,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="16" t="b">
@@ -8354,13 +9070,13 @@
         <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>262</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>263</v>
       </c>
       <c r="E44" s="16" t="b">
         <v>0</v>
@@ -8369,7 +9085,7 @@
     <row r="45" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -8382,10 +9098,10 @@
         <v>38</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16" t="b">
@@ -8397,10 +9113,10 @@
         <v>39</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="16" t="b">
@@ -8412,13 +9128,13 @@
         <v>40</v>
       </c>
       <c r="B48" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D48" s="25" t="s">
         <v>267</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>268</v>
       </c>
       <c r="E48" s="16" t="b">
         <v>0</v>
@@ -8429,10 +9145,10 @@
         <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="16" t="b">
@@ -8485,13 +9201,13 @@
         <v>42</v>
       </c>
       <c r="B50" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>271</v>
       </c>
       <c r="E50" s="16" t="b">
         <v>0</v>
@@ -8502,10 +9218,10 @@
         <v>43</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16" t="b">
@@ -8515,7 +9231,7 @@
     <row r="52" spans="1:46" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -8528,13 +9244,13 @@
         <v>44</v>
       </c>
       <c r="B53" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="E53" s="16" t="b">
         <v>0</v>
@@ -8545,10 +9261,10 @@
         <v>45</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16" t="b">
@@ -8560,13 +9276,13 @@
         <v>46</v>
       </c>
       <c r="B55" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>277</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>278</v>
       </c>
       <c r="E55" s="16" t="b">
         <v>0</v>
@@ -8577,13 +9293,13 @@
         <v>47</v>
       </c>
       <c r="B56" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" s="27" t="s">
         <v>279</v>
-      </c>
-      <c r="C56" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>280</v>
       </c>
       <c r="E56" s="28" t="b">
         <v>0</v>
@@ -8594,10 +9310,10 @@
         <v>48</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="28" t="b">
@@ -8609,10 +9325,10 @@
         <v>49</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="28" t="b">
@@ -8621,10 +9337,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8635,7 +9351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E2CEC-5E0E-48DE-BE54-48780618BFB0}">
   <dimension ref="A1:O35"/>
   <sheetViews>
@@ -8660,7 +9376,7 @@
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
       <c r="B1" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -8668,164 +9384,164 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="32" t="s">
         <v>285</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>286</v>
-      </c>
       <c r="E2" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="C3" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="D3" s="34" t="s">
         <v>289</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>290</v>
       </c>
       <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>292</v>
-      </c>
       <c r="C4" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>289</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>290</v>
       </c>
       <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:8" ht="318.75" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>295</v>
-      </c>
       <c r="D5" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="C6" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="34" t="s">
         <v>298</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>299</v>
       </c>
       <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="C7" s="35" t="s">
         <v>301</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>302</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="D8" s="34" t="s">
         <v>306</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>307</v>
       </c>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>308</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>309</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="C10" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="D10" s="34" t="s">
+      <c r="E10" s="39" t="s">
         <v>313</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="C11" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>316</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>317</v>
       </c>
       <c r="E11" s="39"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -8835,14 +9551,14 @@
     </row>
     <row r="14" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>318</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>319</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="36"/>
@@ -8851,19 +9567,19 @@
     </row>
     <row r="15" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="C15" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E15" s="39" t="s">
         <v>323</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>324</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -8871,19 +9587,19 @@
     </row>
     <row r="16" spans="1:8" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="C16" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>326</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D16" s="34" t="s">
+      <c r="E16" s="39" t="s">
         <v>327</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>328</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -8891,238 +9607,238 @@
     </row>
     <row r="17" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="C17" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D17" s="34" t="s">
+      <c r="E17" s="39" t="s">
         <v>331</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="B18" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="C18" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="C18" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="39" t="s">
         <v>335</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="262.5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="B19" s="73" t="s">
         <v>337</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="C19" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>323</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>339</v>
-      </c>
       <c r="E19" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="B20" s="73" t="s">
         <v>340</v>
       </c>
-      <c r="B20" s="73" t="s">
-        <v>341</v>
-      </c>
       <c r="C20" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="B21" s="74" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="C21" s="34" t="s">
         <v>343</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="D21" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="D21" s="34" t="s">
-        <v>345</v>
-      </c>
       <c r="E21" s="39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" s="73" t="s">
         <v>346</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="C22" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="D22" s="34" t="s">
         <v>348</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>349</v>
       </c>
       <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="73" t="s">
         <v>350</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="C23" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="D23" s="34" t="s">
         <v>352</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>353</v>
       </c>
       <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="B24" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="C24" s="34" t="s">
         <v>355</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>356</v>
-      </c>
       <c r="D24" s="34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="B25" s="73" t="s">
         <v>357</v>
       </c>
-      <c r="B25" s="73" t="s">
-        <v>358</v>
-      </c>
       <c r="C25" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="D25" s="34" t="s">
         <v>352</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>353</v>
       </c>
       <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:15" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26" s="73" t="s">
         <v>359</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="C26" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>361</v>
-      </c>
       <c r="D26" s="34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:15" ht="168.75" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="B27" s="73" t="s">
         <v>362</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="C27" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="D27" s="34" t="s">
         <v>364</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="E27" s="39" t="s">
         <v>365</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
+        <v>366</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>362</v>
+      </c>
+      <c r="C28" s="34" t="s">
         <v>367</v>
       </c>
-      <c r="B28" s="73" t="s">
-        <v>363</v>
-      </c>
-      <c r="C28" s="34" t="s">
+      <c r="D28" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>369</v>
-      </c>
       <c r="E28" s="39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="236.25" x14ac:dyDescent="0.5">
       <c r="A29" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>362</v>
+      </c>
+      <c r="C29" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="B29" s="73" t="s">
-        <v>363</v>
-      </c>
-      <c r="C29" s="34" t="s">
+      <c r="D29" s="34" t="s">
         <v>371</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="E29" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="O29" s="72" t="s">
         <v>372</v>
       </c>
-      <c r="E29" s="39" t="s">
-        <v>366</v>
-      </c>
-      <c r="O29" s="72" t="s">
+    </row>
+    <row r="30" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
+      <c r="B30" s="73" t="s">
+        <v>362</v>
+      </c>
+      <c r="C30" s="34" t="s">
         <v>374</v>
-      </c>
-      <c r="B30" s="73" t="s">
-        <v>363</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>375</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -9130,87 +9846,87 @@
     </row>
     <row r="32" spans="1:15" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="B32" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="C32" s="34" t="s">
         <v>377</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>378</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
+        <v>379</v>
+      </c>
+      <c r="B33" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="C33" s="41" t="s">
         <v>381</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>382</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>381</v>
+      </c>
+      <c r="D34" s="34" t="s">
         <v>383</v>
       </c>
-      <c r="B34" s="41" t="s">
-        <v>381</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>382</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>384</v>
-      </c>
       <c r="E34" s="39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="37" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E30">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F16 F35">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Change project name in eclipse form clientGUIFX to client and server for each sub-project
</commit_message>
<xml_diff>
--- a/BLib_MindMap.xlsx
+++ b/BLib_MindMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/yuval_kogan_e_braude_ac_il/Documents/Documents/Degree/5th Semester/BLib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="587" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C5F914C-F42A-4F63-ACCB-251CEE04B07E}"/>
+  <xr:revisionPtr revIDLastSave="592" documentId="13_ncr:1_{ACD65071-6259-4EC4-BFAF-D28D77085BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA5E7AEF-5F90-444A-8F8C-30FF3F249960}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Task2 - Engineering Methods" sheetId="8" r:id="rId9"/>
     <sheet name="Task2 - Man-Machine Interface" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="476">
   <si>
     <t>Group No. 5</t>
   </si>
@@ -4342,12 +4342,18 @@
   <si>
     <t>Add lecturer to the table</t>
   </si>
+  <si>
+    <t>סיום מטלה 2 של ממשק</t>
+  </si>
+  <si>
+    <t>התחלת עבודה על מימוש הפרויקט הסופי</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5230,6 +5236,167 @@
   </cellStyles>
   <dxfs count="134">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
@@ -5279,34 +5446,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5384,34 +5523,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5556,13 +5667,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5591,6 +5695,13 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5628,78 +5739,22 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -5819,13 +5874,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5843,6 +5891,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5996,13 +6051,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -6022,6 +6070,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -6051,20 +6106,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6092,7 +6133,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6162,13 +6203,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="0"/>
         </left>
@@ -6179,6 +6213,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6216,27 +6257,13 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6310,27 +6337,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6423,66 +6429,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}" name="Table3" displayName="Table3" ref="A2:C17" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
   <autoFilter ref="A2:C17" xr:uid="{05AA9DA6-CC08-4FC9-B206-989554B57B7A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="128" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{4E7545FA-D79C-4E60-9AE2-22B64E4B04C5}" name="Link:" dataDxfId="131" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{FC501C83-E011-46B6-B1B0-80AB0ACB9D4E}" name="Description:" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{B63B935F-466B-475B-A3BA-A840BCF25CB3}" name="Use:" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" headerRowBorderDxfId="50" tableBorderDxfId="51" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}" name="Table6" displayName="Table6" ref="A2:E34" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
   <autoFilter ref="A2:E34" xr:uid="{248AE4E0-9B81-4839-A501-711DDE651122}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{F9395754-A98A-4727-80B4-0D9487FE053E}" name="Test ID" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{1C737D87-3A27-4EDD-893E-18EC87DEB90A}" name="Description" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{A0F4E6C3-5841-411E-9616-BE77FCB000AC}" name="Expected Result" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{0EFC9414-7BF9-49FC-942B-F0519A942264}" name="Precondition" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{29E297FB-DD0A-45BA-AAD1-1305B0D2AD17}" name="Comments" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:H17" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}" name="Table7" displayName="Table7" ref="A1:H17" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:H17" xr:uid="{8C1E50B1-ECE5-44F2-B51F-28135A3F57FC}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{6F08DEB8-9412-4A60-827F-650CE5DE012A}" name="מי עשה בקרה?" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{0B213265-848E-42AD-BB24-FACA108AE82B}" name="עבר בקרה?" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{C212956F-6717-4ACE-9560-C2C858E916CC}" name="ניקוד במטלה" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{4BAEA3F5-7A0E-45FC-BD15-78D20A6CE5AF}" name="הערות" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{B153FC94-978E-4BD3-93BA-8E1FD229FB8C}" name="משימה" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{5FBB8218-0CA9-4720-B017-F7F06795179F}" name="פירוט" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{3B692938-958E-4CEE-ABB6-393545F6D534}" name="זוג מבצע" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{B54BF809-F003-4EE3-9DAB-FF8415660A8A}" name="בוצע?" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{6F08DEB8-9412-4A60-827F-650CE5DE012A}" name="מי עשה בקרה?" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{0B213265-848E-42AD-BB24-FACA108AE82B}" name="עבר בקרה?" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{C212956F-6717-4ACE-9560-C2C858E916CC}" name="ניקוד במטלה" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{4BAEA3F5-7A0E-45FC-BD15-78D20A6CE5AF}" name="הערות" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="J3:K7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}" name="Table12" displayName="Table12" ref="J3:K7" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="J3:K7" xr:uid="{066042A7-5ACA-4CC6-A87D-D9430ED21C10}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9D0FE680-0194-44E8-8173-C409E67F91A6}" name="קישור" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{4D3F5656-E6FB-49EB-ACFD-772E84A9C306}" name="הסבר" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{9D0FE680-0194-44E8-8173-C409E67F91A6}" name="קישור" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{4D3F5656-E6FB-49EB-ACFD-772E84A9C306}" name="הסבר" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C7AC7C6D-F385-46C1-AF38-CDA1CFB529BE}" name="Table11" displayName="Table11" ref="A19:C30" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C7AC7C6D-F385-46C1-AF38-CDA1CFB529BE}" name="Table11" displayName="Table11" ref="A19:C30" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A19:C30" xr:uid="{C7AC7C6D-F385-46C1-AF38-CDA1CFB529BE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{57D5C4F4-64FD-4EFD-808E-E0801EF70843}" name="הערות UML:" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{F806FB25-CBE9-4A56-911B-78A294B244BB}" name="מה לעשות?" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{6769BA36-EFA5-494A-86DC-C52F5A3CBC10}" name="בוצע?" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{57D5C4F4-64FD-4EFD-808E-E0801EF70843}" name="הערות UML:" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{F806FB25-CBE9-4A56-911B-78A294B244BB}" name="מה לעשות?" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{6769BA36-EFA5-494A-86DC-C52F5A3CBC10}" name="בוצע?" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6492,151 +6498,151 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D4EA9A6E-187B-4B46-B60C-FA1D709A52D6}" name="Table14" displayName="Table14" ref="A32:D39" totalsRowShown="0">
   <autoFilter ref="A32:D39" xr:uid="{D4EA9A6E-187B-4B46-B60C-FA1D709A52D6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{72FA54EC-DB57-408F-9F91-B8AA3B826EB1}" name="הערות טיראן" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F8D0778E-1EEE-4D81-BC85-D3139EFF7C4B}" name="מה לעשות?" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{1C407960-B00B-445C-B5EB-A479E02EEB82}" name="בוצע?" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{93A32B96-E1CF-4230-92F0-C1E00651AD0C}" name="תשובות" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{72FA54EC-DB57-408F-9F91-B8AA3B826EB1}" name="הערות טיראן" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{F8D0778E-1EEE-4D81-BC85-D3139EFF7C4B}" name="מה לעשות?" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{1C407960-B00B-445C-B5EB-A479E02EEB82}" name="בוצע?" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{93A32B96-E1CF-4230-92F0-C1E00651AD0C}" name="תשובות" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{987D062A-F148-4472-B909-8204292FB429}" name="Table9" displayName="Table9" ref="A1:A6" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{987D062A-F148-4472-B909-8204292FB429}" name="Table9" displayName="Table9" ref="A1:A6" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:A6" xr:uid="{987D062A-F148-4472-B909-8204292FB429}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{AE01AEED-CFF1-4414-9EAA-6174383BCA7C}" name="Links" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{AE01AEED-CFF1-4414-9EAA-6174383BCA7C}" name="Links" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C95D32FB-859B-4209-80FF-339F84A4F767}" name="Table10" displayName="Table10" ref="C1:E4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C95D32FB-859B-4209-80FF-339F84A4F767}" name="Table10" displayName="Table10" ref="C1:E4" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="C1:E4" xr:uid="{C95D32FB-859B-4209-80FF-339F84A4F767}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EEF69765-8BBA-402D-ADC3-9CDFD9D37FA1}" name="משימה" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{ED6C2DC2-A67D-4080-90BF-59C9DD16DCC2}" name="בוצע?" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{718425F0-840A-4FA7-A37E-5EB58D90FD0F}" name="קישורים" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{EEF69765-8BBA-402D-ADC3-9CDFD9D37FA1}" name="משימה" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{ED6C2DC2-A67D-4080-90BF-59C9DD16DCC2}" name="בוצע?" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{718425F0-840A-4FA7-A37E-5EB58D90FD0F}" name="קישורים" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{0BE04A23-4C0B-47AC-80E2-FA0BA60E805D}" name="Table13" displayName="Table13" ref="C6:F14" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{0BE04A23-4C0B-47AC-80E2-FA0BA60E805D}" name="Table13" displayName="Table13" ref="C6:F14" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="C6:F14" xr:uid="{0BE04A23-4C0B-47AC-80E2-FA0BA60E805D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D6669C51-E03A-4427-9174-DEE960E2B162}" name="Window name:" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{07E70D59-D79F-4B77-AAC5-6C37C7AC65B0}" name="Contains:" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C72C8868-86D2-46D3-B1B1-49EAAB3864A1}" name="Details" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{16A3F3DD-44C8-4331-A29E-2B9047FC9617}" name="Done?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D6669C51-E03A-4427-9174-DEE960E2B162}" name="Window name:" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{07E70D59-D79F-4B77-AAC5-6C37C7AC65B0}" name="Contains:" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{C72C8868-86D2-46D3-B1B1-49EAAB3864A1}" name="Details" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{16A3F3DD-44C8-4331-A29E-2B9047FC9617}" name="Done?" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}" name="Table4" displayName="Table4" ref="E2:I15" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
   <autoFilter ref="E2:I15" xr:uid="{19DDBED5-D056-41C6-879B-F06273FB53FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="119"/>
+    <tableColumn id="1" xr3:uid="{4A44B17B-B413-4495-BB7C-11C4866A56E1}" name="בוצע?" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{B6A1379C-04D7-483C-A304-985079FE316C}" name="שם מטלה" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{5D70691D-166C-4694-B6AE-0ABBE6CCB426}" name="תאריך הגשה" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{C96DA111-E4F1-4D9A-997E-F55F86AA8CB5}" name="הערות" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{0DD43564-66E9-43E5-BF61-68E4F1B24AC8}" name="דחיפות (ימים נותרו להגשה)" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B596997C-7F5E-41C7-9C43-A25E5C965ACB}" name="Table15" displayName="Table15" ref="A1:F9" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" headerRowBorderDxfId="113" tableBorderDxfId="114" totalsRowBorderDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B596997C-7F5E-41C7-9C43-A25E5C965ACB}" name="Table15" displayName="Table15" ref="A1:F9" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118" totalsRowBorderDxfId="117">
   <autoFilter ref="A1:F9" xr:uid="{B596997C-7F5E-41C7-9C43-A25E5C965ACB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{61F8A91C-00CE-4F86-87EC-02E99A6BC410}" name="פירוט" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{F3FD8F8A-6E4B-48A5-8584-D15D1BA3019A}" name="זוג מבצע" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{7A608EA5-0D5F-4B0D-AA3B-FFAE5490AC85}" name="בוצע?" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{81841372-8071-45B2-A912-BE75B2E67CC4}" name="מי עשה בקרה?" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{28F6B4CD-2DE8-49A2-9236-41EB8C723BA6}" name="עבר בקרה?" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{EBB1C6A7-E372-4490-B9D8-B9C8E06457ED}" name="הערות" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{61F8A91C-00CE-4F86-87EC-02E99A6BC410}" name="פירוט" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{F3FD8F8A-6E4B-48A5-8584-D15D1BA3019A}" name="זוג מבצע" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{7A608EA5-0D5F-4B0D-AA3B-FFAE5490AC85}" name="בוצע?" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{81841372-8071-45B2-A912-BE75B2E67CC4}" name="מי עשה בקרה?" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{28F6B4CD-2DE8-49A2-9236-41EB8C723BA6}" name="עבר בקרה?" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{EBB1C6A7-E372-4490-B9D8-B9C8E06457ED}" name="הערות" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{2DC2DFF9-CE45-419F-912B-AAC986CF89FA}" name="Table16" displayName="Table16" ref="H1:I7" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{2DC2DFF9-CE45-419F-912B-AAC986CF89FA}" name="Table16" displayName="Table16" ref="H1:I7" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
   <autoFilter ref="H1:I7" xr:uid="{2DC2DFF9-CE45-419F-912B-AAC986CF89FA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F4361F61-A9EE-4A80-B8B3-8B6A380079C5}" name="Link" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{DD7F5C9A-73B5-46B1-9E78-EB98FBE2C404}" name="Comments" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{F4361F61-A9EE-4A80-B8B3-8B6A380079C5}" name="Link" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{DD7F5C9A-73B5-46B1-9E78-EB98FBE2C404}" name="Comments" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C43" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
-  <autoFilter ref="A1:C43" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}" name="Table8" displayName="Table8" ref="A1:C44" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
+  <autoFilter ref="A1:C44" xr:uid="{81EA5261-0E52-4B64-B8AF-ACB7DC927FB7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{8B68F3F4-DC06-4C70-B802-DE826AF82A24}" name="תאריך פגישה" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{FBA5C8B9-FDE1-40B9-B0A1-44D3B9FF2E0B}" name="מטרת הפגישה" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{4692FF95-B4EB-4D21-8FE4-24648AC3291C}" name="הערות" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="A1:E7" xr:uid="{B35DA877-1B09-46FC-BB9D-741D51916AB5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7DD096F3-29E7-44B9-8E03-74AE8B0EFB58}" name="Full Name" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{86460309-D719-48D5-BE5A-FED925E8C505}" name="תפקיד 1 - שיטות" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{47A50531-CD06-43C3-AF93-5FE6CE915387}" name="תפקיד 2 - שיטות" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{9327F458-CD94-484D-95E0-7A5C295651CA}" name="תפקיד 1 - ממשק אדם - מחשב" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{875991B2-2D2B-439E-AAE3-9B4D6238D1C7}" name="Comments" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{7DD096F3-29E7-44B9-8E03-74AE8B0EFB58}" name="Full Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{86460309-D719-48D5-BE5A-FED925E8C505}" name="תפקיד 1 - שיטות" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{47A50531-CD06-43C3-AF93-5FE6CE915387}" name="תפקיד 2 - שיטות" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{9327F458-CD94-484D-95E0-7A5C295651CA}" name="תפקיד 1 - ממשק אדם - מחשב" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{875991B2-2D2B-439E-AAE3-9B4D6238D1C7}" name="Comments" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:G58" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" headerRowBorderDxfId="84" tableBorderDxfId="85" totalsRowBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}" name="Table1" displayName="Table1" ref="A1:G58" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="A1:G58" xr:uid="{6D424CE2-4373-411D-B684-2BF5A9ABBD05}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{9DB7BAB7-A31F-44B6-803A-703E0BDF2709}" name="Assigned To?" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{F4295F9C-5CAE-4811-8FE0-FF70C50E7BB9}" name="Branch name" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{6956194A-A947-40C0-828D-2186BB183A56}" name="Req. Number" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{20895F69-8ACE-4E61-BA28-80B8C1971A12}" name="Requirement Description" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{4590C1B3-8B8E-4822-BE20-62BB3C89BB06}" name="Req. Type (FR/NFR)" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{85E99892-B63E-4814-8A8B-A75AA4C740C3}" name="comments" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{9DB7BAB7-A31F-44B6-803A-703E0BDF2709}" name="Assigned To?" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{F4295F9C-5CAE-4811-8FE0-FF70C50E7BB9}" name="Branch name" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{5E2A6311-91AA-4D50-94F5-13B5CDDED9B1}" name="Done?" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4D81BCB5-E253-4D33-8DD8-EC35B229DB22}" name="Table118" displayName="Table118" ref="A1:E58" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" headerRowBorderDxfId="72" tableBorderDxfId="73" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4D81BCB5-E253-4D33-8DD8-EC35B229DB22}" name="Table118" displayName="Table118" ref="A1:E58" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A1:E58" xr:uid="{4D81BCB5-E253-4D33-8DD8-EC35B229DB22}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9054BB68-C276-4E7F-A572-060774BCAA32}" name="Test Name" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{DD5D328A-DC77-4C36-BF5C-EEB841317B50}" name="Test Description" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{234EDFF7-FFEB-42D9-835D-6A4BC0EC7332}" name="comments" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{C257F692-1FC5-4509-AA4C-A6DBB914E138}" name="Branch name" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{21A9CEAE-D4D4-4DF5-9F07-E0867982A63E}" name="Done?" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{9054BB68-C276-4E7F-A572-060774BCAA32}" name="Test Name" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{DD5D328A-DC77-4C36-BF5C-EEB841317B50}" name="Test Description" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{234EDFF7-FFEB-42D9-835D-6A4BC0EC7332}" name="comments" dataDxfId="75"/>
+    <tableColumn id="9" xr3:uid="{C257F692-1FC5-4509-AA4C-A6DBB914E138}" name="Branch name" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{21A9CEAE-D4D4-4DF5-9F07-E0867982A63E}" name="Done?" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="63" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A1:C38" xr:uid="{28506447-2809-4030-BABA-9EEC80EDB162}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{09988C74-9D09-4330-8BEF-688D790D1366}" name="Category" dataDxfId="69"/>
     <tableColumn id="2" xr3:uid="{250D87B3-0E0E-41F7-BADF-53EC76930D5E}" name="Specification"/>
     <tableColumn id="3" xr3:uid="{53542E77-0500-4A50-A0B6-226ADBB40CAE}" name="Details"/>
   </tableColumns>
@@ -6942,35 +6948,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E429A24-44E4-45FF-AD25-4F9463F77043}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2"/>
-    <col min="5" max="5" width="9.5703125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="2"/>
+    <col min="5" max="5" width="9.5546875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.28515625" style="2"/>
+    <col min="10" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="65">
         <f ca="1">TODAY()</f>
-        <v>45654</v>
+        <v>45660</v>
       </c>
       <c r="I1" s="61"/>
     </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="21">
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
@@ -6996,7 +7002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.15">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
@@ -7020,10 +7026,10 @@
       </c>
       <c r="I3" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>14</v>
       </c>
@@ -7047,10 +7053,10 @@
       </c>
       <c r="I4" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>19</v>
       </c>
@@ -7067,7 +7073,7 @@
       <c r="G5" s="61"/>
       <c r="I5" s="64"/>
     </row>
-    <row r="6" spans="1:9" ht="100.9">
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>21</v>
       </c>
@@ -7091,7 +7097,7 @@
       </c>
       <c r="I6" s="64"/>
     </row>
-    <row r="7" spans="1:9" ht="28.9">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
         <v>26</v>
       </c>
@@ -7115,10 +7121,10 @@
       </c>
       <c r="I7" s="64">
         <f ca="1">Table4[[#This Row],[תאריך הגשה]]-$G$1</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
         <v>30</v>
       </c>
@@ -7134,7 +7140,7 @@
       <c r="G8" s="61"/>
       <c r="I8" s="64"/>
     </row>
-    <row r="9" spans="1:9" s="47" customFormat="1" ht="18">
+    <row r="9" spans="1:9" s="47" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -7144,7 +7150,7 @@
       <c r="G9" s="62"/>
       <c r="I9" s="64"/>
     </row>
-    <row r="10" spans="1:9" ht="14.45">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="E10" s="58" t="b">
         <v>0</v>
@@ -7153,7 +7159,7 @@
       <c r="G10" s="61"/>
       <c r="I10" s="64"/>
     </row>
-    <row r="11" spans="1:9" ht="18">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
         <v>32</v>
@@ -7166,7 +7172,7 @@
       <c r="G11" s="61"/>
       <c r="I11" s="64"/>
     </row>
-    <row r="12" spans="1:9" ht="28.9">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>33</v>
       </c>
@@ -7179,7 +7185,7 @@
       <c r="G12" s="61"/>
       <c r="I12" s="64"/>
     </row>
-    <row r="13" spans="1:9" ht="14.45">
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>35</v>
       </c>
@@ -7196,7 +7202,7 @@
       <c r="G13" s="61"/>
       <c r="I13" s="64"/>
     </row>
-    <row r="14" spans="1:9" ht="14.45">
+    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>38</v>
       </c>
@@ -7212,7 +7218,7 @@
       <c r="G14" s="61"/>
       <c r="I14" s="64"/>
     </row>
-    <row r="15" spans="1:9" ht="28.9">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>41</v>
       </c>
@@ -7224,109 +7230,109 @@
       </c>
       <c r="G15" s="61"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
       <c r="G16" s="61"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="G17" s="63"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G18" s="61"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G19" s="61"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G20" s="61"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G21" s="61"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G22" s="61"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G23" s="61"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G24" s="61"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G25" s="61"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G26" s="61"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G27" s="61"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G28" s="61"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G29" s="61"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G30" s="61"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G31" s="61"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G32" s="61"/>
     </row>
-    <row r="33" spans="7:7">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" s="61"/>
     </row>
-    <row r="34" spans="7:7">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" s="61"/>
     </row>
-    <row r="35" spans="7:7">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" s="61"/>
     </row>
-    <row r="36" spans="7:7">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" s="61"/>
     </row>
-    <row r="37" spans="7:7">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" s="61"/>
     </row>
-    <row r="38" spans="7:7">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G38" s="61"/>
     </row>
-    <row r="39" spans="7:7">
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G39" s="61"/>
     </row>
-    <row r="40" spans="7:7">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G40" s="61"/>
     </row>
-    <row r="41" spans="7:7">
+    <row r="41" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G41" s="61"/>
     </row>
-    <row r="42" spans="7:7">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G42" s="61"/>
     </row>
-    <row r="43" spans="7:7">
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G43" s="61"/>
     </row>
-    <row r="44" spans="7:7">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G44" s="61"/>
     </row>
-    <row r="45" spans="7:7">
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G45" s="61"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="131" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7376,15 +7382,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="91" t="s">
         <v>448</v>
       </c>
@@ -7398,7 +7404,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="92" t="s">
         <v>450</v>
       </c>
@@ -7412,7 +7418,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="92" t="s">
         <v>452</v>
       </c>
@@ -7426,7 +7432,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="92" t="s">
         <v>455</v>
       </c>
@@ -7440,7 +7446,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="92" t="s">
         <v>458</v>
       </c>
@@ -7448,7 +7454,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="91"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="92" t="s">
         <v>459</v>
       </c>
@@ -7465,7 +7471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="93" t="s">
         <v>454</v>
       </c>
@@ -7480,7 +7486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="172.9">
+    <row r="8" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" s="93" t="s">
         <v>457</v>
       </c>
@@ -7495,7 +7501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72">
+    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="91"/>
       <c r="C9" s="1" t="s">
         <v>466</v>
@@ -7508,7 +7514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="100.9">
+    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="91"/>
       <c r="B10" s="91"/>
       <c r="C10" s="1" t="s">
@@ -7522,7 +7528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="100.9">
+    <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>470</v>
       </c>
@@ -7536,7 +7542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>470</v>
       </c>
@@ -7548,7 +7554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -7556,7 +7562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -7566,18 +7572,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F14">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7609,21 +7615,21 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="118" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="117" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="100" t="s">
         <v>43</v>
       </c>
@@ -7649,7 +7655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1">
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="109"/>
       <c r="B2" s="95" t="s">
         <v>49</v>
@@ -7665,7 +7671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
         <v>51</v>
       </c>
@@ -7687,7 +7693,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
         <v>55</v>
       </c>
@@ -7707,7 +7713,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="110" t="s">
         <v>58</v>
       </c>
@@ -7727,7 +7733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6">
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -7747,7 +7753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.9">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="109"/>
       <c r="B7" s="95" t="s">
         <v>64</v>
@@ -7763,7 +7769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -7779,7 +7785,7 @@
       </c>
       <c r="F8" s="98"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="112" t="s">
         <v>68</v>
       </c>
@@ -7797,10 +7803,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6 E3:E6 C8:C9 E8:E9">
-    <cfRule type="cellIs" dxfId="118" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7820,19 +7826,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1538DB23-0864-46D9-82F7-B6A0E6DA13F2}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="79.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="79.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -7843,7 +7849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="76">
         <v>45617</v>
       </c>
@@ -7852,7 +7858,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="76">
         <v>45619</v>
       </c>
@@ -7861,7 +7867,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="76">
         <v>45622</v>
       </c>
@@ -7870,7 +7876,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="76">
         <v>45624</v>
       </c>
@@ -7879,7 +7885,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="76">
         <v>45625</v>
       </c>
@@ -7888,7 +7894,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="76">
         <v>45628</v>
       </c>
@@ -7897,7 +7903,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="76">
         <v>45630</v>
       </c>
@@ -7906,7 +7912,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="76">
         <v>45635</v>
       </c>
@@ -7915,7 +7921,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="76">
         <v>45636</v>
       </c>
@@ -7924,7 +7930,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="76">
         <v>45638</v>
       </c>
@@ -7933,7 +7939,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="76">
         <v>45639</v>
       </c>
@@ -7942,7 +7948,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="76">
         <v>45640</v>
       </c>
@@ -7951,7 +7957,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="76">
         <v>45643</v>
       </c>
@@ -7960,7 +7966,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="76">
         <v>45650</v>
       </c>
@@ -7969,7 +7975,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="76">
         <v>45652</v>
       </c>
@@ -7978,7 +7984,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="76">
         <v>45654</v>
       </c>
@@ -7987,145 +7993,156 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="76">
-        <v>45657</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>45595</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>474</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="76">
+        <v>45294</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="76">
         <v>45664</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="76">
-        <v>45671</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="76">
-        <v>45678</v>
+        <v>45671</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="76">
-        <v>45685</v>
+        <v>45678</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="76"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="76">
+        <v>45685</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="76"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="76"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="76"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="76"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="76"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="76"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="76"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="76"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="76"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="76"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="76"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="76"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="76"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="76"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="76"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="76"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="76"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="76"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="76"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="76"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="76"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8143,17 +8160,17 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -8170,7 +8187,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.9">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -8185,7 +8202,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>95</v>
       </c>
@@ -8198,7 +8215,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.9">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>98</v>
       </c>
@@ -8211,7 +8228,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.9">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
@@ -8224,7 +8241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>104</v>
       </c>
@@ -8239,7 +8256,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.9">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
@@ -8270,17 +8287,17 @@
       <selection pane="bottomLeft" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="29.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="29.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="7" customFormat="1" ht="21">
+    <row r="1" spans="1:48" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>111</v>
       </c>
@@ -8304,7 +8321,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:48" s="3" customFormat="1" ht="18">
+    <row r="2" spans="1:48" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>118</v>
@@ -8358,7 +8375,7 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -8375,7 +8392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -8392,7 +8409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -8409,7 +8426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:48" ht="43.15">
+    <row r="6" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -8426,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:48">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -8443,7 +8460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:48">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -8460,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:48" s="3" customFormat="1">
+    <row r="9" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -8518,7 +8535,7 @@
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
     </row>
-    <row r="10" spans="1:48" ht="18">
+    <row r="10" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>128</v>
@@ -8531,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>8</v>
       </c>
@@ -8546,7 +8563,7 @@
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="1:48" s="3" customFormat="1" ht="28.9">
+    <row r="12" spans="1:48" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>9</v>
       </c>
@@ -8604,7 +8621,7 @@
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
     </row>
-    <row r="13" spans="1:48" s="3" customFormat="1" ht="43.15">
+    <row r="13" spans="1:48" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>10</v>
       </c>
@@ -8662,7 +8679,7 @@
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
     </row>
-    <row r="14" spans="1:48" ht="43.15">
+    <row r="14" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>11</v>
       </c>
@@ -8679,7 +8696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:48" s="3" customFormat="1" ht="28.9">
+    <row r="15" spans="1:48" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>12</v>
       </c>
@@ -8737,7 +8754,7 @@
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
     </row>
-    <row r="16" spans="1:48" ht="18">
+    <row r="16" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>134</v>
@@ -8750,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:48">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>13</v>
       </c>
@@ -8767,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:48">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>14</v>
       </c>
@@ -8784,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:48">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>15</v>
       </c>
@@ -8801,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:48" ht="28.9">
+    <row r="20" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>16</v>
       </c>
@@ -8818,7 +8835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:48">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>17</v>
       </c>
@@ -8835,7 +8852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:48">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>18</v>
       </c>
@@ -8852,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:48">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>19</v>
       </c>
@@ -8869,7 +8886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:48">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>20</v>
       </c>
@@ -8886,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:48">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>21</v>
       </c>
@@ -8903,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:48">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>22</v>
       </c>
@@ -8920,7 +8937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:48" ht="28.9">
+    <row r="27" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
         <v>23</v>
       </c>
@@ -8937,7 +8954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:48" s="3" customFormat="1" ht="28.9">
+    <row r="28" spans="1:48" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
         <v>24</v>
       </c>
@@ -8995,7 +9012,7 @@
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
     </row>
-    <row r="29" spans="1:48" s="3" customFormat="1">
+    <row r="29" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>25</v>
       </c>
@@ -9053,7 +9070,7 @@
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
     </row>
-    <row r="30" spans="1:48">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
         <v>26</v>
       </c>
@@ -9070,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:48" ht="28.9">
+    <row r="31" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>27</v>
       </c>
@@ -9087,7 +9104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:48" ht="18">
+    <row r="32" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>150</v>
@@ -9100,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:48" ht="28.9">
+    <row r="33" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
         <v>27</v>
       </c>
@@ -9117,7 +9134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:48">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
         <v>28</v>
       </c>
@@ -9134,7 +9151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:48" ht="43.15">
+    <row r="35" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
         <v>29</v>
       </c>
@@ -9153,7 +9170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:48">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
         <v>30</v>
       </c>
@@ -9170,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:48">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
         <v>31</v>
       </c>
@@ -9187,7 +9204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:48" s="4" customFormat="1" ht="28.9">
+    <row r="38" spans="1:48" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
         <v>32</v>
       </c>
@@ -9245,7 +9262,7 @@
       <c r="AU38" s="30"/>
       <c r="AV38" s="30"/>
     </row>
-    <row r="39" spans="1:48" ht="28.9">
+    <row r="39" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
         <v>33</v>
       </c>
@@ -9262,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:48">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <v>34</v>
       </c>
@@ -9279,7 +9296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:48" ht="18">
+    <row r="41" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
         <v>160</v>
@@ -9292,7 +9309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:48" s="4" customFormat="1" ht="18">
+    <row r="42" spans="1:48" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
         <v>35</v>
       </c>
@@ -9350,7 +9367,7 @@
       <c r="AU42" s="30"/>
       <c r="AV42" s="30"/>
     </row>
-    <row r="43" spans="1:48" ht="28.9">
+    <row r="43" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <v>36</v>
       </c>
@@ -9367,7 +9384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:48" ht="28.9">
+    <row r="44" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
         <v>37</v>
       </c>
@@ -9386,7 +9403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:48" ht="18">
+    <row r="45" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
         <v>165</v>
@@ -9399,7 +9416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:48">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
         <v>38</v>
       </c>
@@ -9416,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:48">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
         <v>39</v>
       </c>
@@ -9433,7 +9450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:48" ht="57.6">
+    <row r="48" spans="1:48" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
         <v>40</v>
       </c>
@@ -9452,7 +9469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:48" s="3" customFormat="1">
+    <row r="49" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
         <v>41</v>
       </c>
@@ -9510,7 +9527,7 @@
       <c r="AU49" s="1"/>
       <c r="AV49" s="1"/>
     </row>
-    <row r="50" spans="1:48" ht="28.9">
+    <row r="50" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
         <v>42</v>
       </c>
@@ -9529,7 +9546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:48" ht="28.9">
+    <row r="51" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>43</v>
       </c>
@@ -9546,7 +9563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:48" ht="18">
+    <row r="52" spans="1:48" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
         <v>174</v>
@@ -9559,7 +9576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:48" ht="43.15">
+    <row r="53" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
         <v>44</v>
       </c>
@@ -9578,7 +9595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:48">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <v>45</v>
       </c>
@@ -9595,7 +9612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:48" ht="28.9">
+    <row r="55" spans="1:48" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
         <v>46</v>
       </c>
@@ -9614,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:48" ht="43.15">
+    <row r="56" spans="1:48" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="26">
         <v>47</v>
       </c>
@@ -9633,7 +9650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:48">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="26">
         <v>48</v>
       </c>
@@ -9650,7 +9667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:48">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" s="26">
         <v>49</v>
       </c>
@@ -9669,10 +9686,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="89" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9694,15 +9711,15 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="29.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>184</v>
       </c>
@@ -9719,7 +9736,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>118</v>
@@ -9730,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -9739,7 +9756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -9748,7 +9765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -9757,7 +9774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -9766,7 +9783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="17"/>
@@ -9775,7 +9792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="17"/>
@@ -9784,7 +9801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -9793,7 +9810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>128</v>
@@ -9804,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="15" t="s">
         <v>129</v>
@@ -9813,7 +9830,7 @@
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" ht="28.9">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
         <v>130</v>
@@ -9824,7 +9841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.15">
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
         <v>131</v>
@@ -9835,7 +9852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="43.15">
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
         <v>132</v>
@@ -9846,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.9">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
         <v>133</v>
@@ -9857,7 +9874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>134</v>
@@ -9868,7 +9885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
         <v>135</v>
@@ -9879,7 +9896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
         <v>136</v>
@@ -9890,7 +9907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="68" t="s">
         <v>137</v>
@@ -9901,7 +9918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.9">
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
         <v>138</v>
@@ -9912,7 +9929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
         <v>139</v>
@@ -9923,7 +9940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
         <v>140</v>
@@ -9934,7 +9951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
         <v>141</v>
@@ -9945,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="15" t="s">
         <v>142</v>
@@ -9956,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15" t="s">
         <v>143</v>
@@ -9967,7 +9984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="15" t="s">
         <v>144</v>
@@ -9978,7 +9995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.9">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="15" t="s">
         <v>145</v>
@@ -9989,7 +10006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.9">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
         <v>146</v>
@@ -10000,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15" t="s">
         <v>147</v>
@@ -10011,7 +10028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="15" t="s">
         <v>148</v>
@@ -10022,7 +10039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.9">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="15" t="s">
         <v>149</v>
@@ -10033,7 +10050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18">
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>150</v>
@@ -10044,7 +10061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.9">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="15" t="s">
         <v>151</v>
@@ -10055,7 +10072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="15" t="s">
         <v>152</v>
@@ -10066,7 +10083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.15">
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="15" t="s">
         <v>153</v>
@@ -10079,7 +10096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="15" t="s">
         <v>155</v>
@@ -10090,7 +10107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="15" t="s">
         <v>156</v>
@@ -10101,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.9">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="15" t="s">
         <v>157</v>
@@ -10112,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="28.9">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="15" t="s">
         <v>158</v>
@@ -10123,7 +10140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="15" t="s">
         <v>159</v>
@@ -10134,7 +10151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="18">
+    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="11" t="s">
         <v>160</v>
@@ -10145,7 +10162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="15" t="s">
         <v>161</v>
@@ -10156,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.9">
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="15" t="s">
         <v>162</v>
@@ -10167,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.9">
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="15" t="s">
         <v>163</v>
@@ -10180,7 +10197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18">
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
       <c r="B45" s="11" t="s">
         <v>165</v>
@@ -10191,7 +10208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="B46" s="15" t="s">
         <v>166</v>
@@ -10202,7 +10219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="15" t="s">
         <v>167</v>
@@ -10213,7 +10230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="57.6">
+    <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15" t="s">
         <v>168</v>
@@ -10226,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="15" t="s">
         <v>170</v>
@@ -10237,7 +10254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="28.9">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="15" t="s">
         <v>171</v>
@@ -10250,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.9">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="15" t="s">
         <v>173</v>
@@ -10261,7 +10278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="18">
+    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
         <v>174</v>
@@ -10272,7 +10289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="43.15">
+    <row r="53" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="15" t="s">
         <v>175</v>
@@ -10285,7 +10302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="14"/>
       <c r="B54" s="15" t="s">
         <v>177</v>
@@ -10296,7 +10313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="28.9">
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
       <c r="B55" s="15" t="s">
         <v>178</v>
@@ -10309,7 +10326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="43.15">
+    <row r="56" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
       <c r="B56" s="27" t="s">
         <v>180</v>
@@ -10322,7 +10339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="26"/>
       <c r="B57" s="71" t="s">
         <v>182</v>
@@ -10333,7 +10350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="26"/>
       <c r="B58" s="71" t="s">
         <v>183</v>
@@ -10360,14 +10377,14 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>186</v>
       </c>
@@ -10378,7 +10395,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
         <v>189</v>
       </c>
@@ -10389,7 +10406,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
         <v>189</v>
       </c>
@@ -10400,7 +10417,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>189</v>
       </c>
@@ -10411,7 +10428,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="55" t="s">
         <v>189</v>
       </c>
@@ -10422,7 +10439,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
         <v>189</v>
       </c>
@@ -10433,7 +10450,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="55" t="s">
         <v>189</v>
       </c>
@@ -10444,7 +10461,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="56" t="s">
         <v>202</v>
       </c>
@@ -10455,7 +10472,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
         <v>202</v>
       </c>
@@ -10466,7 +10483,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
         <v>202</v>
       </c>
@@ -10477,7 +10494,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="56" t="s">
         <v>202</v>
       </c>
@@ -10488,7 +10505,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
         <v>202</v>
       </c>
@@ -10499,7 +10516,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="55" t="s">
         <v>213</v>
       </c>
@@ -10510,7 +10527,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="55" t="s">
         <v>213</v>
       </c>
@@ -10521,7 +10538,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="55" t="s">
         <v>213</v>
       </c>
@@ -10532,7 +10549,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="55" t="s">
         <v>213</v>
       </c>
@@ -10543,7 +10560,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="55" t="s">
         <v>213</v>
       </c>
@@ -10554,7 +10571,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="55" t="s">
         <v>213</v>
       </c>
@@ -10565,7 +10582,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="56" t="s">
         <v>226</v>
       </c>
@@ -10576,7 +10593,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
         <v>226</v>
       </c>
@@ -10587,7 +10604,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="56" t="s">
         <v>226</v>
       </c>
@@ -10598,7 +10615,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="55" t="s">
         <v>233</v>
       </c>
@@ -10609,7 +10626,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
         <v>233</v>
       </c>
@@ -10620,7 +10637,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="56" t="s">
         <v>233</v>
       </c>
@@ -10631,7 +10648,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="56" t="s">
         <v>233</v>
       </c>
@@ -10642,7 +10659,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="56" t="s">
         <v>240</v>
       </c>
@@ -10653,7 +10670,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="56" t="s">
         <v>240</v>
       </c>
@@ -10664,7 +10681,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="56" t="s">
         <v>240</v>
       </c>
@@ -10675,7 +10692,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="56" t="s">
         <v>240</v>
       </c>
@@ -10686,7 +10703,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="55" t="s">
         <v>249</v>
       </c>
@@ -10697,7 +10714,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="55" t="s">
         <v>249</v>
       </c>
@@ -10708,7 +10725,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="55" t="s">
         <v>249</v>
       </c>
@@ -10719,7 +10736,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="55" t="s">
         <v>249</v>
       </c>
@@ -10730,7 +10747,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="56" t="s">
         <v>258</v>
       </c>
@@ -10741,7 +10758,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="56" t="s">
         <v>258</v>
       </c>
@@ -10752,7 +10769,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="55" t="s">
         <v>263</v>
       </c>
@@ -10763,7 +10780,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="55" t="s">
         <v>263</v>
       </c>
@@ -10774,7 +10791,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="55" t="s">
         <v>263</v>
       </c>
@@ -10801,21 +10818,21 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="66" style="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="36" customWidth="1"/>
     <col min="3" max="3" width="27" style="30" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="30" customWidth="1"/>
     <col min="5" max="5" width="20" style="30" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="30"/>
+    <col min="6" max="6" width="9.33203125" style="30"/>
     <col min="7" max="7" width="45" style="30" customWidth="1"/>
-    <col min="8" max="14" width="9.28515625" style="30"/>
-    <col min="15" max="15" width="70.140625" style="30" customWidth="1"/>
-    <col min="16" max="16384" width="9.28515625" style="30"/>
+    <col min="8" max="14" width="9.33203125" style="30"/>
+    <col min="15" max="15" width="70.109375" style="30" customWidth="1"/>
+    <col min="16" max="16384" width="9.33203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.45">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="49"/>
       <c r="B1" s="42" t="s">
         <v>128</v>
@@ -10824,7 +10841,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>270</v>
       </c>
@@ -10841,7 +10858,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
         <v>274</v>
       </c>
@@ -10856,7 +10873,7 @@
       </c>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" spans="1:8" ht="90">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
         <v>278</v>
       </c>
@@ -10871,7 +10888,7 @@
       </c>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:8" ht="306">
+    <row r="5" spans="1:8" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>280</v>
       </c>
@@ -10886,7 +10903,7 @@
       </c>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" spans="1:8" ht="108">
+    <row r="6" spans="1:8" ht="108" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>283</v>
       </c>
@@ -10901,7 +10918,7 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:8" ht="90">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
         <v>287</v>
       </c>
@@ -10916,7 +10933,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="90">
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>291</v>
       </c>
@@ -10931,7 +10948,7 @@
       </c>
       <c r="E8" s="39"/>
     </row>
-    <row r="9" spans="1:8" ht="90">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
         <v>295</v>
       </c>
@@ -10948,7 +10965,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="90">
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A10" s="38" t="s">
         <v>298</v>
       </c>
@@ -10965,7 +10982,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="108">
+    <row r="11" spans="1:8" ht="108" x14ac:dyDescent="0.3">
       <c r="A11" s="38" t="s">
         <v>302</v>
       </c>
@@ -10980,7 +10997,7 @@
       </c>
       <c r="E11" s="39"/>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1">
+    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>134</v>
@@ -10991,7 +11008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="234">
+    <row r="14" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
         <v>305</v>
       </c>
@@ -11007,7 +11024,7 @@
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
     </row>
-    <row r="15" spans="1:8" ht="234">
+    <row r="15" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A15" s="38" t="s">
         <v>308</v>
       </c>
@@ -11027,7 +11044,7 @@
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
     </row>
-    <row r="16" spans="1:8" ht="234">
+    <row r="16" spans="1:8" ht="234" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
         <v>312</v>
       </c>
@@ -11047,7 +11064,7 @@
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
     </row>
-    <row r="17" spans="1:15" ht="234">
+    <row r="17" spans="1:15" ht="234" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
         <v>316</v>
       </c>
@@ -11064,7 +11081,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="234">
+    <row r="18" spans="1:15" ht="234" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>320</v>
       </c>
@@ -11081,7 +11098,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="234">
+    <row r="19" spans="1:15" ht="234" x14ac:dyDescent="0.3">
       <c r="A19" s="38" t="s">
         <v>324</v>
       </c>
@@ -11098,7 +11115,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="108">
+    <row r="20" spans="1:15" ht="108" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
         <v>327</v>
       </c>
@@ -11115,7 +11132,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="108">
+    <row r="21" spans="1:15" ht="108" x14ac:dyDescent="0.3">
       <c r="A21" s="38" t="s">
         <v>329</v>
       </c>
@@ -11133,7 +11150,7 @@
       </c>
       <c r="G21" s="34"/>
     </row>
-    <row r="22" spans="1:15" ht="72">
+    <row r="22" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="38" t="s">
         <v>333</v>
       </c>
@@ -11148,7 +11165,7 @@
       </c>
       <c r="E22" s="39"/>
     </row>
-    <row r="23" spans="1:15" ht="72">
+    <row r="23" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="38" t="s">
         <v>337</v>
       </c>
@@ -11163,7 +11180,7 @@
       </c>
       <c r="E23" s="39"/>
     </row>
-    <row r="24" spans="1:15" ht="36">
+    <row r="24" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>341</v>
       </c>
@@ -11178,7 +11195,7 @@
       </c>
       <c r="E24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="72">
+    <row r="25" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
         <v>344</v>
       </c>
@@ -11193,7 +11210,7 @@
       </c>
       <c r="E25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="54">
+    <row r="26" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>346</v>
       </c>
@@ -11208,7 +11225,7 @@
       </c>
       <c r="E26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="162">
+    <row r="27" spans="1:15" ht="162" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="s">
         <v>349</v>
       </c>
@@ -11225,7 +11242,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="108">
+    <row r="28" spans="1:15" ht="108" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>354</v>
       </c>
@@ -11242,7 +11259,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="235.15">
+    <row r="29" spans="1:15" ht="235.2" x14ac:dyDescent="0.65">
       <c r="A29" s="38" t="s">
         <v>357</v>
       </c>
@@ -11262,7 +11279,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="72">
+    <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
         <v>361</v>
       </c>
@@ -11277,7 +11294,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
         <v>174</v>
@@ -11286,7 +11303,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="75"/>
     </row>
-    <row r="32" spans="1:15" ht="72">
+    <row r="32" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>363</v>
       </c>
@@ -11301,7 +11318,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="90">
+    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A33" s="52" t="s">
         <v>367</v>
       </c>
@@ -11316,7 +11333,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="90">
+    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A34" s="38" t="s">
         <v>370</v>
       </c>
@@ -11333,7 +11350,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="37" customFormat="1" ht="23.45">
+    <row r="35" spans="1:5" s="37" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
         <v>372</v>
@@ -11341,34 +11358,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E30">
-    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F16 F35">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"NFR"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"FR"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11387,26 +11404,26 @@
       <selection activeCell="B1" sqref="B1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.42578125" style="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="78" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="78" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="78" customWidth="1"/>
+    <col min="1" max="1" width="68.6640625" style="78" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.44140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="78" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="78" customWidth="1"/>
     <col min="7" max="7" width="16" style="78" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" style="86" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="86" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="79" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.28515625" style="79" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="78"/>
+    <col min="9" max="9" width="20.109375" style="86" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="79" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" style="79" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="78"/>
     <col min="13" max="13" width="14" style="78" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="78" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="78"/>
+    <col min="14" max="14" width="21.44140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>373</v>
       </c>
@@ -11439,7 +11456,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.9">
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="83"/>
       <c r="C2" s="80" t="s">
@@ -11458,7 +11475,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="43.15">
+    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>379</v>
       </c>
@@ -11489,7 +11506,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1">
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>385</v>
       </c>
@@ -11519,7 +11536,7 @@
       </c>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="100.9">
+    <row r="5" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -11550,7 +11567,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="28.9">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>394</v>
       </c>
@@ -11581,7 +11598,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="43.15">
+    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>398</v>
       </c>
@@ -11610,7 +11627,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="57.6">
+    <row r="8" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>402</v>
       </c>
@@ -11637,7 +11654,7 @@
       </c>
       <c r="I8" s="84"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="83"/>
       <c r="C9" s="80" t="s">
@@ -11651,13 +11668,13 @@
       <c r="I9" s="84"/>
       <c r="J9" s="90">
         <f ca="1">'Important Information'!I4</f>
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K9" s="89" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="28.9">
+    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>408</v>
       </c>
@@ -11678,7 +11695,7 @@
       <c r="H10" s="84"/>
       <c r="I10" s="84"/>
     </row>
-    <row r="11" spans="1:15" ht="72">
+    <row r="11" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>410</v>
       </c>
@@ -11697,7 +11714,7 @@
       <c r="H11" s="84"/>
       <c r="I11" s="84"/>
     </row>
-    <row r="12" spans="1:15" ht="72">
+    <row r="12" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="85" t="s">
         <v>412</v>
@@ -11714,7 +11731,7 @@
       <c r="H12" s="84"/>
       <c r="I12" s="84"/>
     </row>
-    <row r="13" spans="1:15" ht="28.9">
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>413</v>
       </c>
@@ -11733,7 +11750,7 @@
       <c r="H13" s="84"/>
       <c r="I13" s="84"/>
     </row>
-    <row r="14" spans="1:15" ht="57.6">
+    <row r="14" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>415</v>
       </c>
@@ -11754,7 +11771,7 @@
       </c>
       <c r="I14" s="85"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="83"/>
       <c r="C15" s="3" t="s">
@@ -11767,7 +11784,7 @@
       <c r="H15" s="87"/>
       <c r="I15" s="84"/>
     </row>
-    <row r="16" spans="1:15" ht="57.6">
+    <row r="16" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>392</v>
       </c>
@@ -11790,7 +11807,7 @@
       <c r="H16" s="84"/>
       <c r="I16" s="84"/>
     </row>
-    <row r="17" spans="1:12" ht="43.15">
+    <row r="17" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>396</v>
       </c>
@@ -11815,7 +11832,7 @@
       </c>
       <c r="I17" s="84"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -11825,7 +11842,7 @@
       <c r="H18" s="84"/>
       <c r="I18" s="84"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>423</v>
       </c>
@@ -11836,7 +11853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="57.6">
+    <row r="20" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>425</v>
       </c>
@@ -11847,7 +11864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>427</v>
       </c>
@@ -11858,7 +11875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28.9">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>429</v>
       </c>
@@ -11872,7 +11889,7 @@
       <c r="J22" s="86"/>
       <c r="L22" s="79"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>431</v>
       </c>
@@ -11886,7 +11903,7 @@
       <c r="J23" s="86"/>
       <c r="L23" s="79"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>433</v>
       </c>
@@ -11900,7 +11917,7 @@
       <c r="J24" s="86"/>
       <c r="L24" s="79"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>435</v>
       </c>
@@ -11914,7 +11931,7 @@
       <c r="J25" s="86"/>
       <c r="L25" s="79"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>436</v>
       </c>
@@ -11928,7 +11945,7 @@
       <c r="J26" s="86"/>
       <c r="L26" s="79"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>437</v>
       </c>
@@ -11942,7 +11959,7 @@
       <c r="J27" s="86"/>
       <c r="L27" s="79"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="88" t="b">
@@ -11952,7 +11969,7 @@
       <c r="J28" s="86"/>
       <c r="L28" s="79"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>439</v>
       </c>
@@ -11964,7 +11981,7 @@
       <c r="J29" s="86"/>
       <c r="L29" s="79"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>440</v>
       </c>
@@ -11976,12 +11993,12 @@
       <c r="J30" s="86"/>
       <c r="L30" s="79"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H31" s="78"/>
       <c r="J31" s="86"/>
       <c r="L31" s="79"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>441</v>
       </c>
@@ -11998,7 +12015,7 @@
       <c r="J32" s="86"/>
       <c r="L32" s="79"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>443</v>
       </c>
@@ -12009,7 +12026,7 @@
       <c r="J33" s="86"/>
       <c r="L33" s="79"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>444</v>
       </c>
@@ -12020,7 +12037,7 @@
       <c r="J34" s="86"/>
       <c r="L34" s="79"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>445</v>
       </c>
@@ -12032,7 +12049,7 @@
       <c r="J35" s="86"/>
       <c r="L35" s="79"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>446</v>
       </c>
@@ -12044,7 +12061,7 @@
       <c r="J36" s="86"/>
       <c r="L36" s="79"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>447</v>
       </c>
@@ -12056,7 +12073,7 @@
       <c r="J37" s="86"/>
       <c r="L37" s="79"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="84"/>
@@ -12066,7 +12083,7 @@
       <c r="J38" s="86"/>
       <c r="L38" s="79"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="84"/>
@@ -12076,7 +12093,7 @@
       <c r="J39" s="86"/>
       <c r="L39" s="79"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="84"/>
@@ -12086,7 +12103,7 @@
       <c r="J40" s="86"/>
       <c r="L40" s="79"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="84"/>
@@ -12096,7 +12113,7 @@
       <c r="J41" s="86"/>
       <c r="L41" s="79"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="84"/>
@@ -12106,7 +12123,7 @@
       <c r="J42" s="86"/>
       <c r="L42" s="79"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="84"/>
@@ -12116,7 +12133,7 @@
       <c r="J43" s="86"/>
       <c r="L43" s="79"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="84"/>
@@ -12126,7 +12143,7 @@
       <c r="J44" s="86"/>
       <c r="L44" s="79"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="84"/>
@@ -12136,7 +12153,7 @@
       <c r="J45" s="86"/>
       <c r="L45" s="79"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="84"/>
@@ -12146,7 +12163,7 @@
       <c r="J46" s="86"/>
       <c r="L46" s="79"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="84"/>
@@ -12159,18 +12176,18 @@
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
   <conditionalFormatting sqref="C20:C30">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8 F3:F8 D10:D14 F10:F14 D16:D17 F16:F17">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>